<commit_message>
Rewrote ASM encode function
</commit_message>
<xml_diff>
--- a/performance/performance.xlsx
+++ b/performance/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Kitzan\Documents\GitHub\seng440-huffman-coding\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EC77E8-720D-495E-8A39-E017EEEA3B29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9321FE76-D4DA-4A6A-8E51-E8ACE0C230F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21495" yWindow="2535" windowWidth="18300" windowHeight="7455" activeTab="2" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="17">
   <si>
     <t>Percentage</t>
   </si>
@@ -82,6 +82,9 @@
   <si>
     <t>Subject</t>
   </si>
+  <si>
+    <t>Functional Unit</t>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -256,58 +259,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -338,39 +301,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -380,6 +310,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,7 +1011,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$6:$C$8</c:f>
+              <c:f>Aggregate!$C$7:$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1016,7 +1028,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$D$6:$D$8</c:f>
+              <c:f>Aggregate!$D$7:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1064,7 +1076,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$6:$C$8</c:f>
+              <c:f>Aggregate!$C$7:$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1081,7 +1093,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$E$6:$E$8</c:f>
+              <c:f>Aggregate!$E$7:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1129,7 +1141,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$6:$C$8</c:f>
+              <c:f>Aggregate!$C$7:$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1146,7 +1158,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$F$6:$F$8</c:f>
+              <c:f>Aggregate!$F$7:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1498,7 +1510,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$9:$C$11</c:f>
+              <c:f>Aggregate!$C$11:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1515,7 +1527,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$D$9:$D$11</c:f>
+              <c:f>Aggregate!$D$11:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1563,7 +1575,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$9:$C$11</c:f>
+              <c:f>Aggregate!$C$11:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1580,7 +1592,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$E$9:$E$11</c:f>
+              <c:f>Aggregate!$E$11:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1628,7 +1640,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$9:$C$11</c:f>
+              <c:f>Aggregate!$C$11:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1645,7 +1657,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$F$9:$F$11</c:f>
+              <c:f>Aggregate!$F$11:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1997,7 +2009,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$12:$C$14</c:f>
+              <c:f>Aggregate!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2014,7 +2026,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$D$12:$D$14</c:f>
+              <c:f>Aggregate!$D$15:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2062,7 +2074,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$12:$C$14</c:f>
+              <c:f>Aggregate!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2079,7 +2091,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$E$12:$E$14</c:f>
+              <c:f>Aggregate!$E$15:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2127,7 +2139,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Aggregate!$C$12:$C$14</c:f>
+              <c:f>Aggregate!$C$15:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2144,7 +2156,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Aggregate!$F$12:$F$14</c:f>
+              <c:f>Aggregate!$F$15:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -5014,13 +5026,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55E637-485C-412D-B940-A453CA463644}">
   <dimension ref="B2:L39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" customWidth="1"/>
@@ -5030,173 +5042,173 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="26" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="27">
         <v>8031625000</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="29">
         <v>0.14065</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="30">
         <f>_xlfn.CEILING.MATH(D3*F3)</f>
         <v>1129648057</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="29">
         <v>0.40057500000000001</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="30">
         <f>_xlfn.CEILING.MATH(D3*F4)</f>
         <v>3217268185</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="4" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="35">
         <f>1-F3-F4</f>
         <v>0.45877500000000004</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="36">
         <f>_xlfn.CEILING.MATH(D3*F5)</f>
         <v>3684708760</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="36"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="38">
         <v>10975812500</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="29">
         <v>0.111375</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="30">
         <f>_xlfn.CEILING.MATH(D6*F6)</f>
         <v>1222431118</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="29">
         <v>0.53992499999999999</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="30">
         <f>_xlfn.CEILING.MATH(D6*F7)</f>
         <v>5926115565</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="4" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="35">
         <f>1-F6-F7</f>
         <v>0.34870000000000001</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="36">
         <f>_xlfn.CEILING.MATH(D6*F8)</f>
         <v>3827265819</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="36"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="38">
         <v>15213125000</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="40">
         <v>7.3925000000000005E-2</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="30">
         <f>_xlfn.CEILING.MATH(D9*F9)</f>
         <v>1124630266</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="29">
         <v>0.61262499999999998</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="30">
         <f>_xlfn.CEILING.MATH(D9*F10)</f>
         <v>9319940704</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="6" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="43">
         <f>1-F9-F10</f>
         <v>0.31345000000000001</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="44">
         <f>_xlfn.CEILING.MATH(D9*F11)</f>
         <v>4768554032</v>
       </c>
@@ -5206,22 +5218,22 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="27">
         <v>6658937500</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="29">
         <v>0.161</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="30">
         <f>_xlfn.CEILING.MATH(D12*F12)</f>
         <v>1072088938</v>
       </c>
@@ -5231,16 +5243,16 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="29">
         <v>0.25074999999999997</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="30">
         <f>_xlfn.CEILING.MATH(D12*F13)</f>
         <v>1669728579</v>
       </c>
@@ -5250,79 +5262,79 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="4" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="35">
         <f>1-F12-F13</f>
         <v>0.58824999999999994</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="36">
         <f>_xlfn.CEILING.MATH(D12*F14)</f>
         <v>3917119985</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="21"/>
+      <c r="J14" s="10"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="36"/>
-      <c r="C15" s="35" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="38">
         <v>7234250000</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="29">
         <v>0.12847500000000001</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="30">
         <f>_xlfn.CEILING.MATH(D15*F15)</f>
         <v>929420269</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="21"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="29">
         <v>0.43422500000000003</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="30">
         <f>_xlfn.CEILING.MATH(D15*F16)</f>
         <v>3141292207</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="21"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="4" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="35">
         <f>1-F15-F16</f>
         <v>0.43729999999999997</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="36">
         <f>_xlfn.CEILING.MATH(D15*F17)</f>
         <v>3163537525</v>
       </c>
@@ -5332,20 +5344,20 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="36"/>
-      <c r="C18" s="35" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="38">
         <v>11646625000</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="40">
         <v>8.5349999999999995E-2</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="30">
         <f>_xlfn.CEILING.MATH(D18*F18)</f>
         <v>994039444</v>
       </c>
@@ -5355,16 +5367,16 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="3" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="29">
         <v>0.52117500000000005</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="30">
         <f>_xlfn.CEILING.MATH(D18*F19)</f>
         <v>6069929785</v>
       </c>
@@ -5374,229 +5386,313 @@
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="6" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="43">
         <f>1-F18-F19</f>
         <v>0.39347499999999991</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="44">
         <f>_xlfn.CEILING.MATH(D18*F20)</f>
         <v>4582655772</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="27">
         <v>6294375000</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="29">
         <v>0.14197499999999999</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="30">
         <f>_xlfn.CEILING.MATH(D21*F21)</f>
         <v>893643891</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="3" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="29">
         <v>0.30924499999999999</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="30">
         <f>_xlfn.CEILING.MATH(D21*F22)</f>
         <v>1946503997</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="36"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="4" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="35">
         <f>1-F21-F22</f>
         <v>0.54878000000000005</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="36">
         <f>_xlfn.CEILING.MATH(D21*F23)</f>
         <v>3454227113</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="36"/>
-      <c r="C24" s="35" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="38">
         <v>6577687500</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="29">
         <v>0.151425</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="30">
         <f>_xlfn.CEILING.MATH(D24*F24)</f>
         <v>996026330</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="3" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="29">
         <v>0.31190000000000001</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="30">
         <f>_xlfn.CEILING.MATH(D24*F25)</f>
         <v>2051580732</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="36"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="4" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="45">
         <f>1-F24-F25</f>
         <v>0.53667500000000001</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="36">
         <f>_xlfn.CEILING.MATH(D24*F26)</f>
         <v>3530080440</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="36"/>
-      <c r="C27" s="35" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="38">
         <v>7765437500</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="40">
         <v>0.13272500000000001</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="30">
         <f>_xlfn.CEILING.MATH(D27*F27)</f>
         <v>1030667693</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="3" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="29">
         <v>0.27712500000000001</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="30">
         <f>_xlfn.CEILING.MATH(D27*F28)</f>
         <v>2151996868</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="6" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="46">
         <f>1-F27-F28</f>
         <v>0.59014999999999995</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="44">
         <f>_xlfn.CEILING.MATH(D27*F29)</f>
         <v>4582772941</v>
       </c>
     </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B30" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30">
+        <f>_xlfn.CEILING.MATH(D30*F30)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="1"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30">
+        <f>_xlfn.CEILING.MATH(D30*F31)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="24"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="35"/>
+      <c r="G32" s="36">
+        <f>_xlfn.CEILING.MATH(D30*F32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="24"/>
+      <c r="C33" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="38"/>
+      <c r="E33" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30">
+        <f>_xlfn.CEILING.MATH(D33*F33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="30">
+        <f>_xlfn.CEILING.MATH(D33*F34)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="24"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="45"/>
+      <c r="G35" s="36">
+        <f>_xlfn.CEILING.MATH(D33*F35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" s="24"/>
+      <c r="C36" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="40"/>
+      <c r="G36" s="30">
+        <f>_xlfn.CEILING.MATH(D36*F36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="29"/>
+      <c r="G37" s="30">
+        <f>_xlfn.CEILING.MATH(D36*F37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="46"/>
+      <c r="G38" s="44">
+        <f>_xlfn.CEILING.MATH(D36*F38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="2"/>
       <c r="F39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="28">
+    <mergeCell ref="B30:B38"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
     <mergeCell ref="B21:B29"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C15:C17"/>
@@ -5626,17 +5722,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA985C3-79B9-4317-B4D1-8FEF996B666A}">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="9.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
     <col min="5" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.36328125" style="1" customWidth="1"/>
@@ -5645,431 +5741,467 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="22"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="18">
         <f>Performance!D3</f>
         <v>8031625000</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="18">
         <f>Performance!D6</f>
         <v>10975812500</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="19">
         <f>Performance!D9</f>
         <v>15213125000</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="28" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="17">
         <f>Performance!D12</f>
         <v>6658937500</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="17">
         <f>Performance!D15</f>
         <v>7234250000</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="15">
         <f>Performance!D18</f>
         <v>11646625000</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="44"/>
-      <c r="C5" s="31" t="s">
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="21"/>
+      <c r="C5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="47">
         <f>Performance!D21</f>
         <v>6294375000</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="48">
         <f>Performance!D24</f>
         <v>6577687500</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <f>Performance!D27</f>
         <v>7765437500</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="22"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D7" s="18">
         <f>Performance!G3</f>
         <v>1129648057</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E7" s="18">
         <f>Performance!G6</f>
         <v>1222431118</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F7" s="19">
         <f>Performance!G9</f>
         <v>1124630266</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="43"/>
-      <c r="C7" s="28" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="21"/>
+      <c r="C8" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D8" s="17">
         <f>Performance!G12</f>
         <v>1072088938</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E8" s="17">
         <f>Performance!G15</f>
         <v>929420269</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F8" s="15">
         <f>Performance!G18</f>
         <v>994039444</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="44"/>
-      <c r="C8" s="31" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="21"/>
+      <c r="C9" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D9" s="48">
         <f>Performance!G21</f>
         <v>893643891</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E9" s="47">
         <f>Performance!G24</f>
         <v>996026330</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F9" s="3">
         <f>Performance!G27</f>
         <v>1030667693</v>
       </c>
-      <c r="G8" s="20"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="42" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="22"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D11" s="18">
         <f>Performance!G4</f>
         <v>3217268185</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E11" s="18">
         <f>Performance!G7</f>
         <v>5926115565</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F11" s="19">
         <f>Performance!G10</f>
         <v>9319940704</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="43"/>
-      <c r="C10" s="28" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="21"/>
+      <c r="C12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D12" s="17">
         <f>Performance!G13</f>
         <v>1669728579</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E12" s="17">
         <f>Performance!G16</f>
         <v>3141292207</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F12" s="15">
         <f>Performance!G19</f>
         <v>6069929785</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44"/>
-      <c r="C11" s="31" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="21"/>
+      <c r="C13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D13" s="47">
         <f>Performance!G22</f>
         <v>1946503997</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E13" s="47">
         <f>Performance!G25</f>
         <v>2051580732</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F13" s="3">
         <f>Performance!G28</f>
         <v>2151996868</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="19"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="42" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="22"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D15" s="18">
         <f>Performance!G5</f>
         <v>3684708760</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E15" s="18">
         <f>Performance!G8</f>
         <v>3827265819</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F15" s="19">
         <f>Performance!G11</f>
         <v>4768554032</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="43"/>
-      <c r="C13" s="28" t="s">
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" s="21"/>
+      <c r="C16" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D16" s="17">
         <f>Performance!G14</f>
         <v>3917119985</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E16" s="17">
         <f>Performance!G17</f>
         <v>3163537525</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F16" s="15">
         <f>Performance!G20</f>
         <v>4582655772</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="44"/>
-      <c r="C14" s="31" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="21"/>
+      <c r="C17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D17" s="48">
         <f>Performance!G23</f>
         <v>3454227113</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E17" s="48">
         <f>Performance!G26</f>
         <v>3530080440</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F17" s="3">
         <f>Performance!G29</f>
         <v>4582772941</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="22"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
       <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="F43" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B7:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6080,8 +6212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894D5C8D-F7D4-420C-ADAD-D25C20CEEE3B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Computed performance gains from asm optimizations
</commit_message>
<xml_diff>
--- a/performance/performance.xlsx
+++ b/performance/performance.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Kitzan\Documents\GitHub\seng440-huffman-coding\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD616A6D-64C5-4678-BC40-A84A769E2277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51387C2A-50F1-4F25-BB29-FDC16D89BB82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="2" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
     <sheet name="Aggregate" sheetId="2" r:id="rId2"/>
     <sheet name="Charts" sheetId="3" r:id="rId3"/>
-    <sheet name="Encode Opt" sheetId="4" r:id="rId4"/>
-    <sheet name="Decode Opt" sheetId="5" r:id="rId5"/>
+    <sheet name="Optimization" sheetId="8" r:id="rId4"/>
+    <sheet name="Encode OPT" sheetId="4" r:id="rId5"/>
     <sheet name="Encode GCC" sheetId="7" r:id="rId6"/>
-    <sheet name="Decode GCC" sheetId="6" r:id="rId7"/>
+    <sheet name="Decode OPT" sheetId="5" r:id="rId7"/>
+    <sheet name="Decode GCC" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="158">
   <si>
     <t>Percentage</t>
   </si>
@@ -481,6 +482,36 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>OPT</t>
+  </si>
+  <si>
+    <t>GCC</t>
+  </si>
+  <si>
+    <t>27(n)+23</t>
+  </si>
+  <si>
+    <t>Improvement</t>
+  </si>
+  <si>
+    <t>257(n)+11</t>
+  </si>
+  <si>
+    <t>184(n)+28</t>
+  </si>
+  <si>
+    <t>34(n)+30</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>n = char</t>
+  </si>
+  <si>
+    <t>n = uint32</t>
   </si>
 </sst>
 </file>
@@ -490,7 +521,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,8 +552,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -535,8 +573,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -732,12 +776,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -884,6 +941,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5520,7 +5586,7 @@
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D23"/>
+      <selection activeCell="C27" sqref="C27:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6218,7 +6284,7 @@
   <dimension ref="A2:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6705,8 +6771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894D5C8D-F7D4-420C-ADAD-D25C20CEEE3B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6717,11 +6783,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BC710D-19AA-4D12-98C6-2B8F098B36A0}">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" customWidth="1"/>
+    <col min="3" max="3" width="7.90625" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="74">
+        <v>0.2059</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="73" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="75"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="74">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="73" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC2F0A2A-A4D3-4AD5-A5E5-5C9211B027B2}">
   <dimension ref="A1:BK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7055,6 +7214,12 @@
       <c r="L9" t="s">
         <v>45</v>
       </c>
+      <c r="M9" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" t="s">
+        <v>45</v>
+      </c>
       <c r="O9" t="s">
         <v>46</v>
       </c>
@@ -7078,6 +7243,12 @@
         <v>44</v>
       </c>
       <c r="M10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
+      </c>
+      <c r="O10" t="s">
         <v>45</v>
       </c>
       <c r="P10" t="s">
@@ -7099,10 +7270,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="44"/>
-      <c r="M11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" t="s">
         <v>45</v>
       </c>
       <c r="Q11" t="s">
@@ -7123,9 +7294,7 @@
       <c r="B12" s="45">
         <v>1</v>
       </c>
-      <c r="C12" s="44">
-        <v>17</v>
-      </c>
+      <c r="C12" s="44"/>
       <c r="D12" s="40"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
@@ -7136,14 +7305,14 @@
       <c r="K12" s="40"/>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
-      <c r="N12" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="O12" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="R12" s="40" t="s">
         <v>46</v>
       </c>
@@ -7262,6 +7431,9 @@
       <c r="H16" t="s">
         <v>45</v>
       </c>
+      <c r="I16" t="s">
+        <v>45</v>
+      </c>
       <c r="J16" t="s">
         <v>46</v>
       </c>
@@ -7286,6 +7458,9 @@
         <v>44</v>
       </c>
       <c r="I17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" t="s">
         <v>45</v>
       </c>
       <c r="K17" t="s">
@@ -7308,10 +7483,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="44"/>
-      <c r="I18" t="s">
-        <v>44</v>
-      </c>
       <c r="J18" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" t="s">
         <v>45</v>
       </c>
       <c r="L18" t="s">
@@ -7334,10 +7509,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="J19" t="s">
-        <v>44</v>
-      </c>
       <c r="K19" t="s">
+        <v>44</v>
+      </c>
+      <c r="L19" t="s">
         <v>45</v>
       </c>
       <c r="M19" t="s">
@@ -7360,10 +7535,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="44"/>
-      <c r="K20" t="s">
-        <v>44</v>
-      </c>
       <c r="L20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" t="s">
         <v>45</v>
       </c>
       <c r="N20" t="s">
@@ -7389,10 +7564,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="L21" t="s">
-        <v>44</v>
-      </c>
       <c r="M21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" t="s">
         <v>45</v>
       </c>
       <c r="P21" t="s">
@@ -7415,10 +7593,19 @@
         <v>1</v>
       </c>
       <c r="C22" s="44"/>
-      <c r="M22" t="s">
-        <v>44</v>
-      </c>
       <c r="N22" t="s">
+        <v>44</v>
+      </c>
+      <c r="O22" t="s">
+        <v>44</v>
+      </c>
+      <c r="P22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" t="s">
         <v>45</v>
       </c>
       <c r="S22" t="s">
@@ -7442,10 +7629,16 @@
         <v>1</v>
       </c>
       <c r="C23" s="44"/>
-      <c r="N23" t="s">
-        <v>44</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>44</v>
+      </c>
+      <c r="R23" t="s">
+        <v>44</v>
+      </c>
+      <c r="S23" t="s">
         <v>45</v>
       </c>
       <c r="T23" t="s">
@@ -7474,10 +7667,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="44"/>
-      <c r="O24" t="s">
-        <v>44</v>
-      </c>
-      <c r="P24" t="s">
+      <c r="S24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" t="s">
         <v>45</v>
       </c>
       <c r="U24" t="s">
@@ -7508,14 +7701,21 @@
         <v>1</v>
       </c>
       <c r="C25" s="44"/>
-      <c r="P25" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>45</v>
-      </c>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
+      <c r="T25" t="s">
+        <v>44</v>
+      </c>
+      <c r="U25" t="s">
+        <v>45</v>
+      </c>
+      <c r="V25" t="s">
+        <v>45</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X25" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="Y25" s="1" t="s">
         <v>46</v>
       </c>
@@ -7537,9 +7737,7 @@
       <c r="B26" s="45">
         <v>3</v>
       </c>
-      <c r="C26" s="44">
-        <v>27</v>
-      </c>
+      <c r="C26" s="44"/>
       <c r="D26" s="40"/>
       <c r="E26" s="40"/>
       <c r="F26" s="40"/>
@@ -7553,19 +7751,25 @@
       <c r="N26" s="40"/>
       <c r="O26" s="40"/>
       <c r="P26" s="40"/>
-      <c r="Q26" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="R26" s="40" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
       <c r="S26" s="40"/>
       <c r="T26" s="40"/>
-      <c r="U26" s="40"/>
-      <c r="V26" s="41"/>
-      <c r="W26" s="40"/>
-      <c r="X26" s="40"/>
-      <c r="Y26" s="40"/>
+      <c r="U26" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="V26" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="W26" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="X26" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y26" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="Z26" s="40" t="s">
         <v>46</v>
       </c>
@@ -7617,9 +7821,7 @@
       <c r="B28" s="45">
         <v>1</v>
       </c>
-      <c r="C28" s="44">
-        <v>6</v>
-      </c>
+      <c r="C28" s="44"/>
       <c r="D28" s="46"/>
       <c r="E28" s="40" t="s">
         <v>44</v>
@@ -7665,12 +7867,1786 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F74B2D-652B-4E3A-A8D3-572CE0B18B69}">
+  <dimension ref="A1:AG46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="4" max="33" width="2.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="54">
+        <v>1</v>
+      </c>
+      <c r="E1" s="53">
+        <v>2</v>
+      </c>
+      <c r="F1" s="53">
+        <v>3</v>
+      </c>
+      <c r="G1" s="53">
+        <v>4</v>
+      </c>
+      <c r="H1" s="53">
+        <v>5</v>
+      </c>
+      <c r="I1" s="53">
+        <v>6</v>
+      </c>
+      <c r="J1" s="53">
+        <v>7</v>
+      </c>
+      <c r="K1" s="53">
+        <v>8</v>
+      </c>
+      <c r="L1" s="53">
+        <v>9</v>
+      </c>
+      <c r="M1" s="53">
+        <v>10</v>
+      </c>
+      <c r="N1" s="53">
+        <v>11</v>
+      </c>
+      <c r="O1" s="53">
+        <v>12</v>
+      </c>
+      <c r="P1" s="53">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="53">
+        <v>14</v>
+      </c>
+      <c r="R1" s="53">
+        <v>15</v>
+      </c>
+      <c r="S1" s="53">
+        <v>16</v>
+      </c>
+      <c r="T1" s="53">
+        <v>17</v>
+      </c>
+      <c r="U1" s="53">
+        <v>18</v>
+      </c>
+      <c r="V1" s="53">
+        <v>19</v>
+      </c>
+      <c r="W1" s="53">
+        <v>20</v>
+      </c>
+      <c r="X1" s="51">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="42">
+        <v>1</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
+        <v>146</v>
+      </c>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="42">
+        <v>1</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" t="s">
+        <v>146</v>
+      </c>
+      <c r="X3" s="42"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
+      <c r="J4" t="s">
+        <v>146</v>
+      </c>
+      <c r="X4" s="42"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="42">
+        <v>1</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" t="s">
+        <v>146</v>
+      </c>
+      <c r="X5" s="42"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A6" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L6" t="s">
+        <v>146</v>
+      </c>
+      <c r="X6" s="42"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="43">
+        <v>3</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A8" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="42">
+        <v>1</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H8" t="s">
+        <v>146</v>
+      </c>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
+      <c r="AF8" s="11"/>
+      <c r="AG8" s="11"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A9" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="42">
+        <v>1</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9" t="s">
+        <v>146</v>
+      </c>
+      <c r="X9" s="42"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
+      <c r="AF9" s="11"/>
+      <c r="AG9" s="11"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A10" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="42">
+        <v>1</v>
+      </c>
+      <c r="D10" s="49"/>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" t="s">
+        <v>146</v>
+      </c>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
+      <c r="AG10" s="11"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A11" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="42">
+        <v>1</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X11" s="42"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="11"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="11"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A12" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="42">
+        <v>1</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L12" t="s">
+        <v>146</v>
+      </c>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="11"/>
+      <c r="AC12" s="11"/>
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="11"/>
+      <c r="AG12" s="11"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="43">
+        <v>1</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="M13" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="11"/>
+      <c r="AC13" s="11"/>
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="11"/>
+      <c r="AF13" s="11"/>
+      <c r="AG13" s="11"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="42">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H14" t="s">
+        <v>146</v>
+      </c>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="11"/>
+      <c r="AG14" s="11"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A15" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="42">
+        <v>1</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" t="s">
+        <v>147</v>
+      </c>
+      <c r="K15" t="s">
+        <v>146</v>
+      </c>
+      <c r="X15" s="42"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A16" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="42">
+        <v>1</v>
+      </c>
+      <c r="D16" s="49"/>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" t="s">
+        <v>146</v>
+      </c>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A17" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="42">
+        <v>1</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="I17" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" t="s">
+        <v>147</v>
+      </c>
+      <c r="O17" t="s">
+        <v>146</v>
+      </c>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="11"/>
+      <c r="AC17" s="11"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="11"/>
+      <c r="AG17" s="11"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A18" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="42">
+        <v>2</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="L18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" t="s">
+        <v>46</v>
+      </c>
+      <c r="O18" t="s">
+        <v>46</v>
+      </c>
+      <c r="P18" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>146</v>
+      </c>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
+      <c r="AG18" s="11"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A19" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="42">
+        <v>1</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="M19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>147</v>
+      </c>
+      <c r="R19" t="s">
+        <v>146</v>
+      </c>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A20" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="42">
+        <v>1</v>
+      </c>
+      <c r="D20" s="49"/>
+      <c r="N20" t="s">
+        <v>44</v>
+      </c>
+      <c r="O20" t="s">
+        <v>44</v>
+      </c>
+      <c r="P20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>45</v>
+      </c>
+      <c r="R20" t="s">
+        <v>45</v>
+      </c>
+      <c r="S20" t="s">
+        <v>46</v>
+      </c>
+      <c r="T20" t="s">
+        <v>147</v>
+      </c>
+      <c r="U20" t="s">
+        <v>146</v>
+      </c>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
+      <c r="AG20" s="11"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A21" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="43">
+        <v>3</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q21" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="S21" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="U21" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="V21" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="W21" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="X21" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
+      <c r="AG21" s="11"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A22" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="42">
+        <v>1</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" t="s">
+        <v>146</v>
+      </c>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
+      <c r="AG22" s="11"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A23" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="42">
+        <v>1</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" t="s">
+        <v>147</v>
+      </c>
+      <c r="I23" t="s">
+        <v>146</v>
+      </c>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
+      <c r="AG23" s="11"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A24" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="42">
+        <v>1</v>
+      </c>
+      <c r="D24" s="49"/>
+      <c r="F24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="11"/>
+      <c r="AG24" s="11"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A25" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="42">
+        <v>1</v>
+      </c>
+      <c r="D25" s="49"/>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" t="s">
+        <v>147</v>
+      </c>
+      <c r="M25" t="s">
+        <v>146</v>
+      </c>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="11"/>
+      <c r="AG25" s="11"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A26" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="42">
+        <v>1</v>
+      </c>
+      <c r="D26" s="49"/>
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" t="s">
+        <v>46</v>
+      </c>
+      <c r="M26" t="s">
+        <v>147</v>
+      </c>
+      <c r="N26" t="s">
+        <v>146</v>
+      </c>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
+      <c r="AG26" s="11"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A27" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="42">
+        <v>1</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="K27" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" t="s">
+        <v>147</v>
+      </c>
+      <c r="O27" t="s">
+        <v>146</v>
+      </c>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
+      <c r="AG27" s="11"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A28" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="42">
+        <v>1</v>
+      </c>
+      <c r="D28" s="49"/>
+      <c r="L28" t="s">
+        <v>44</v>
+      </c>
+      <c r="M28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N28" t="s">
+        <v>46</v>
+      </c>
+      <c r="O28" t="s">
+        <v>147</v>
+      </c>
+      <c r="P28" t="s">
+        <v>146</v>
+      </c>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="11"/>
+      <c r="Z28" s="11"/>
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="11"/>
+      <c r="AC28" s="11"/>
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="11"/>
+      <c r="AF28" s="11"/>
+      <c r="AG28" s="11"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A29" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="42">
+        <v>1</v>
+      </c>
+      <c r="D29" s="49"/>
+      <c r="M29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29" t="s">
+        <v>46</v>
+      </c>
+      <c r="P29" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>146</v>
+      </c>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="11"/>
+      <c r="Z29" s="11"/>
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="11"/>
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="11"/>
+      <c r="AF29" s="11"/>
+      <c r="AG29" s="11"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="43">
+        <v>3</v>
+      </c>
+      <c r="D30" s="46"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="O30" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="P30" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q30" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="R30" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="S30" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="T30" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="U30" s="40"/>
+      <c r="V30" s="40"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="43"/>
+      <c r="Y30" s="11"/>
+      <c r="Z30" s="11"/>
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="11"/>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="11"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A31" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="42">
+        <v>1</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" t="s">
+        <v>146</v>
+      </c>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="11"/>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="11"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A32" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="42">
+        <v>1</v>
+      </c>
+      <c r="D32" s="49"/>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
+        <v>147</v>
+      </c>
+      <c r="I32" t="s">
+        <v>146</v>
+      </c>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="11"/>
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="11"/>
+      <c r="AF32" s="11"/>
+      <c r="AG32" s="11"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A33" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="43">
+        <v>3</v>
+      </c>
+      <c r="D33" s="46"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="L33" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="43"/>
+      <c r="Y33" s="11"/>
+      <c r="Z33" s="11"/>
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="11"/>
+      <c r="AD33" s="11"/>
+      <c r="AE33" s="11"/>
+      <c r="AF33" s="11"/>
+      <c r="AG33" s="11"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A34" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="42">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="11"/>
+      <c r="AG34" s="11"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A35" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="42">
+        <v>1</v>
+      </c>
+      <c r="D35" s="49"/>
+      <c r="E35" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="11"/>
+      <c r="AF35" s="11"/>
+      <c r="AG35" s="11"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A36" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="42">
+        <v>1</v>
+      </c>
+      <c r="D36" s="49"/>
+      <c r="F36" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="11"/>
+      <c r="AG36" s="11"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A37" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="42">
+        <v>1</v>
+      </c>
+      <c r="D37" s="49"/>
+      <c r="G37" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A38" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="43">
+        <v>3</v>
+      </c>
+      <c r="D38" s="46"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="J38" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="K38" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="L38" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="M38" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="N38" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="O38" s="40"/>
+      <c r="P38" s="40"/>
+      <c r="Q38" s="40"/>
+      <c r="R38" s="40"/>
+      <c r="S38" s="40"/>
+      <c r="T38" s="40"/>
+      <c r="U38" s="40"/>
+      <c r="V38" s="40"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="43"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
+      <c r="AE38" s="11"/>
+      <c r="AF38" s="11"/>
+      <c r="AG38" s="11"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A39" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="42">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="11"/>
+      <c r="AG39" s="11"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A40" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="43">
+        <v>1</v>
+      </c>
+      <c r="D40" s="46"/>
+      <c r="E40" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="I40" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="40"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="40"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="40"/>
+      <c r="R40" s="40"/>
+      <c r="S40" s="40"/>
+      <c r="T40" s="40"/>
+      <c r="U40" s="40"/>
+      <c r="V40" s="40"/>
+      <c r="W40" s="40"/>
+      <c r="X40" s="43"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="11"/>
+      <c r="AD40" s="11"/>
+      <c r="AE40" s="11"/>
+      <c r="AF40" s="11"/>
+      <c r="AG40" s="11"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A41" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="42">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="11"/>
+      <c r="AD41" s="11"/>
+      <c r="AE41" s="11"/>
+      <c r="AF41" s="11"/>
+      <c r="AG41" s="11"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A42" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="11"/>
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="11"/>
+      <c r="AF42" s="11"/>
+      <c r="AG42" s="11"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A43" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="42">
+        <v>1</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="F43" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="11"/>
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="11"/>
+      <c r="AE43" s="11"/>
+      <c r="AF43" s="11"/>
+      <c r="AG43" s="11"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A44" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="43">
+        <v>1</v>
+      </c>
+      <c r="D44" s="46"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="K44" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="40"/>
+      <c r="R44" s="40"/>
+      <c r="S44" s="40"/>
+      <c r="T44" s="40"/>
+      <c r="U44" s="40"/>
+      <c r="V44" s="40"/>
+      <c r="W44" s="40"/>
+      <c r="X44" s="43"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="11"/>
+      <c r="AC44" s="11"/>
+      <c r="AD44" s="11"/>
+      <c r="AE44" s="11"/>
+      <c r="AF44" s="11"/>
+      <c r="AG44" s="11"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="11"/>
+      <c r="AF45" s="11"/>
+      <c r="AG45" s="11"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="11"/>
+      <c r="AC46" s="11"/>
+      <c r="AD46" s="11"/>
+      <c r="AE46" s="11"/>
+      <c r="AF46" s="11"/>
+      <c r="AG46" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E3818A-D03F-4D14-9726-3113DF885761}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8013,9 +9989,6 @@
       </c>
       <c r="B10" s="45">
         <v>1</v>
-      </c>
-      <c r="C10">
-        <v>13</v>
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="40"/>
@@ -8555,9 +10528,6 @@
       </c>
       <c r="B27" s="45">
         <v>3</v>
-      </c>
-      <c r="C27">
-        <v>24</v>
       </c>
       <c r="D27" s="46"/>
       <c r="E27" s="40"/>
@@ -8581,7 +10551,9 @@
       <c r="U27" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="V27" s="40"/>
+      <c r="V27" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="W27" s="40" t="s">
         <v>46</v>
       </c>
@@ -8699,9 +10671,6 @@
       <c r="B31" s="45">
         <v>2</v>
       </c>
-      <c r="C31">
-        <v>11</v>
-      </c>
       <c r="D31" s="46"/>
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
@@ -8711,20 +10680,20 @@
       <c r="H31" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="I31" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="40" t="s">
+        <v>46</v>
+      </c>
       <c r="K31" s="40" t="s">
-        <v>46</v>
+        <v>147</v>
       </c>
       <c r="L31" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M31" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="N31" s="40" t="s">
-        <v>146</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
       <c r="O31" s="40"/>
       <c r="P31" s="40"/>
       <c r="Q31" s="40"/>
@@ -8871,10 +10840,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="45">
-        <v>2</v>
-      </c>
-      <c r="C36">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D36" s="46"/>
       <c r="E36" s="40"/>
@@ -8893,12 +10859,14 @@
         <v>46</v>
       </c>
       <c r="L36" s="40" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="M36" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="N36" s="40"/>
+        <v>147</v>
+      </c>
+      <c r="N36" s="40" t="s">
+        <v>146</v>
+      </c>
       <c r="O36" s="40"/>
       <c r="P36" s="40"/>
       <c r="Q36" s="40"/>
@@ -8924,9 +10892,6 @@
       </c>
       <c r="B37" s="48">
         <v>1</v>
-      </c>
-      <c r="C37">
-        <v>5</v>
       </c>
       <c r="D37" s="46" t="s">
         <v>44</v>
@@ -8973,1758 +10938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F74B2D-652B-4E3A-A8D3-572CE0B18B69}">
-  <dimension ref="A1:AG46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
-    <col min="4" max="33" width="2.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="54">
-        <v>1</v>
-      </c>
-      <c r="E1" s="53">
-        <v>2</v>
-      </c>
-      <c r="F1" s="53">
-        <v>3</v>
-      </c>
-      <c r="G1" s="53">
-        <v>4</v>
-      </c>
-      <c r="H1" s="53">
-        <v>5</v>
-      </c>
-      <c r="I1" s="53">
-        <v>6</v>
-      </c>
-      <c r="J1" s="53">
-        <v>7</v>
-      </c>
-      <c r="K1" s="53">
-        <v>8</v>
-      </c>
-      <c r="L1" s="53">
-        <v>9</v>
-      </c>
-      <c r="M1" s="53">
-        <v>10</v>
-      </c>
-      <c r="N1" s="53">
-        <v>11</v>
-      </c>
-      <c r="O1" s="53">
-        <v>12</v>
-      </c>
-      <c r="P1" s="53">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="53">
-        <v>14</v>
-      </c>
-      <c r="R1" s="53">
-        <v>15</v>
-      </c>
-      <c r="S1" s="53">
-        <v>16</v>
-      </c>
-      <c r="T1" s="53">
-        <v>17</v>
-      </c>
-      <c r="U1" s="53">
-        <v>18</v>
-      </c>
-      <c r="V1" s="53">
-        <v>19</v>
-      </c>
-      <c r="W1" s="53">
-        <v>20</v>
-      </c>
-      <c r="X1" s="51">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="42">
-        <v>1</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H2" t="s">
-        <v>146</v>
-      </c>
-      <c r="X2" s="42"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="49"/>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I3" t="s">
-        <v>146</v>
-      </c>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="11"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="42">
-        <v>1</v>
-      </c>
-      <c r="D4" s="49"/>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J4" t="s">
-        <v>146</v>
-      </c>
-      <c r="X4" s="42"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="42">
-        <v>1</v>
-      </c>
-      <c r="D5" s="49"/>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" t="s">
-        <v>147</v>
-      </c>
-      <c r="K5" t="s">
-        <v>146</v>
-      </c>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" t="s">
-        <v>147</v>
-      </c>
-      <c r="L6" t="s">
-        <v>146</v>
-      </c>
-      <c r="X6" s="42"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="43">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="O7" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="11"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="11"/>
-      <c r="AG7" s="11"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A8" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="42">
-        <v>1</v>
-      </c>
-      <c r="D8" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" t="s">
-        <v>146</v>
-      </c>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="42">
-        <v>1</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9" t="s">
-        <v>146</v>
-      </c>
-      <c r="X9" s="42"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A10" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="42">
-        <v>1</v>
-      </c>
-      <c r="D10" s="49"/>
-      <c r="F10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" t="s">
-        <v>147</v>
-      </c>
-      <c r="J10" t="s">
-        <v>146</v>
-      </c>
-      <c r="X10" s="42"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="42">
-        <v>1</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" s="42">
-        <v>1</v>
-      </c>
-      <c r="D12" s="49"/>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" t="s">
-        <v>147</v>
-      </c>
-      <c r="L12" t="s">
-        <v>146</v>
-      </c>
-      <c r="X12" s="42"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="43">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="M13" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="N13" s="40"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="40"/>
-      <c r="W13" s="40"/>
-      <c r="X13" s="43"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="42">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" t="s">
-        <v>147</v>
-      </c>
-      <c r="H14" t="s">
-        <v>146</v>
-      </c>
-      <c r="X14" s="42"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A15" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B15" s="42">
-        <v>1</v>
-      </c>
-      <c r="D15" s="49"/>
-      <c r="E15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" t="s">
-        <v>147</v>
-      </c>
-      <c r="K15" t="s">
-        <v>146</v>
-      </c>
-      <c r="X15" s="42"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="42">
-        <v>1</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="F16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" t="s">
-        <v>45</v>
-      </c>
-      <c r="L16" t="s">
-        <v>46</v>
-      </c>
-      <c r="M16" t="s">
-        <v>147</v>
-      </c>
-      <c r="N16" t="s">
-        <v>146</v>
-      </c>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A17" s="42" t="s">
-        <v>120</v>
-      </c>
-      <c r="B17" s="42">
-        <v>1</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-      <c r="M17" t="s">
-        <v>46</v>
-      </c>
-      <c r="N17" t="s">
-        <v>147</v>
-      </c>
-      <c r="O17" t="s">
-        <v>146</v>
-      </c>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A18" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="B18" s="42">
-        <v>2</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-      <c r="N18" t="s">
-        <v>46</v>
-      </c>
-      <c r="O18" t="s">
-        <v>46</v>
-      </c>
-      <c r="P18" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>146</v>
-      </c>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A19" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" s="42">
-        <v>1</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="I19" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" t="s">
-        <v>45</v>
-      </c>
-      <c r="P19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>147</v>
-      </c>
-      <c r="R19" t="s">
-        <v>146</v>
-      </c>
-      <c r="X19" s="42"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
-      <c r="AG19" s="11"/>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A20" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="42">
-        <v>1</v>
-      </c>
-      <c r="D20" s="49"/>
-      <c r="J20" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" t="s">
-        <v>45</v>
-      </c>
-      <c r="S20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T20" t="s">
-        <v>147</v>
-      </c>
-      <c r="U20" t="s">
-        <v>146</v>
-      </c>
-      <c r="X20" s="42"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
-      <c r="AD20" s="11"/>
-      <c r="AE20" s="11"/>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A21" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="43">
-        <v>3</v>
-      </c>
-      <c r="C21">
-        <v>21</v>
-      </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="L21" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="40"/>
-      <c r="T21" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="U21" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="V21" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="W21" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="X21" s="43" t="s">
-        <v>146</v>
-      </c>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A22" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22" s="42">
-        <v>1</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" t="s">
-        <v>146</v>
-      </c>
-      <c r="X22" s="42"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="42">
-        <v>1</v>
-      </c>
-      <c r="D23" s="49"/>
-      <c r="E23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" t="s">
-        <v>147</v>
-      </c>
-      <c r="I23" t="s">
-        <v>146</v>
-      </c>
-      <c r="X23" s="42"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
-      <c r="AB23" s="11"/>
-      <c r="AC23" s="11"/>
-      <c r="AD23" s="11"/>
-      <c r="AE23" s="11"/>
-      <c r="AF23" s="11"/>
-      <c r="AG23" s="11"/>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A24" s="42" t="s">
-        <v>126</v>
-      </c>
-      <c r="B24" s="42">
-        <v>1</v>
-      </c>
-      <c r="D24" s="49"/>
-      <c r="F24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" t="s">
-        <v>146</v>
-      </c>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-      <c r="AE24" s="11"/>
-      <c r="AF24" s="11"/>
-      <c r="AG24" s="11"/>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A25" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="42">
-        <v>1</v>
-      </c>
-      <c r="D25" s="49"/>
-      <c r="G25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" t="s">
-        <v>147</v>
-      </c>
-      <c r="M25" t="s">
-        <v>146</v>
-      </c>
-      <c r="X25" s="42"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
-      <c r="AD25" s="11"/>
-      <c r="AE25" s="11"/>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11"/>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A26" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="42">
-        <v>1</v>
-      </c>
-      <c r="D26" s="49"/>
-      <c r="H26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" t="s">
-        <v>46</v>
-      </c>
-      <c r="M26" t="s">
-        <v>147</v>
-      </c>
-      <c r="N26" t="s">
-        <v>146</v>
-      </c>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
-      <c r="AB26" s="11"/>
-      <c r="AC26" s="11"/>
-      <c r="AD26" s="11"/>
-      <c r="AE26" s="11"/>
-      <c r="AF26" s="11"/>
-      <c r="AG26" s="11"/>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A27" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="42">
-        <v>1</v>
-      </c>
-      <c r="D27" s="49"/>
-      <c r="I27" t="s">
-        <v>44</v>
-      </c>
-      <c r="J27" t="s">
-        <v>45</v>
-      </c>
-      <c r="M27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" t="s">
-        <v>147</v>
-      </c>
-      <c r="O27" t="s">
-        <v>146</v>
-      </c>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-      <c r="AD27" s="11"/>
-      <c r="AE27" s="11"/>
-      <c r="AF27" s="11"/>
-      <c r="AG27" s="11"/>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A28" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="B28" s="42">
-        <v>1</v>
-      </c>
-      <c r="D28" s="49"/>
-      <c r="J28" t="s">
-        <v>44</v>
-      </c>
-      <c r="K28" t="s">
-        <v>45</v>
-      </c>
-      <c r="N28" t="s">
-        <v>46</v>
-      </c>
-      <c r="O28" t="s">
-        <v>147</v>
-      </c>
-      <c r="P28" t="s">
-        <v>146</v>
-      </c>
-      <c r="X28" s="42"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
-      <c r="AC28" s="11"/>
-      <c r="AD28" s="11"/>
-      <c r="AE28" s="11"/>
-      <c r="AF28" s="11"/>
-      <c r="AG28" s="11"/>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A29" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="B29" s="42">
-        <v>1</v>
-      </c>
-      <c r="D29" s="49"/>
-      <c r="K29" t="s">
-        <v>44</v>
-      </c>
-      <c r="L29" t="s">
-        <v>45</v>
-      </c>
-      <c r="O29" t="s">
-        <v>46</v>
-      </c>
-      <c r="P29" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>146</v>
-      </c>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
-      <c r="AE29" s="11"/>
-      <c r="AF29" s="11"/>
-      <c r="AG29" s="11"/>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A30" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="43">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>17</v>
-      </c>
-      <c r="D30" s="46"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="M30" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q30" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="R30" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="S30" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="T30" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="U30" s="40"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="40"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
-      <c r="AB30" s="11"/>
-      <c r="AC30" s="11"/>
-      <c r="AD30" s="11"/>
-      <c r="AE30" s="11"/>
-      <c r="AF30" s="11"/>
-      <c r="AG30" s="11"/>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A31" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="42">
-        <v>1</v>
-      </c>
-      <c r="D31" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" t="s">
-        <v>45</v>
-      </c>
-      <c r="F31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H31" t="s">
-        <v>146</v>
-      </c>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="11"/>
-      <c r="AB31" s="11"/>
-      <c r="AC31" s="11"/>
-      <c r="AD31" s="11"/>
-      <c r="AE31" s="11"/>
-      <c r="AF31" s="11"/>
-      <c r="AG31" s="11"/>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A32" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="42">
-        <v>1</v>
-      </c>
-      <c r="D32" s="49"/>
-      <c r="E32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" t="s">
-        <v>45</v>
-      </c>
-      <c r="I32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J32" t="s">
-        <v>147</v>
-      </c>
-      <c r="K32" t="s">
-        <v>146</v>
-      </c>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-      <c r="AE32" s="11"/>
-      <c r="AF32" s="11"/>
-      <c r="AG32" s="11"/>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B33" s="43">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>11</v>
-      </c>
-      <c r="D33" s="46"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="K33" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="L33" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M33" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="N33" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="O33" s="40"/>
-      <c r="P33" s="40"/>
-      <c r="Q33" s="40"/>
-      <c r="R33" s="40"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="40"/>
-      <c r="U33" s="40"/>
-      <c r="V33" s="40"/>
-      <c r="W33" s="40"/>
-      <c r="X33" s="43"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
-      <c r="AG33" s="11"/>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A34" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="42">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>144</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H34" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X34" s="42"/>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="11"/>
-      <c r="AB34" s="11"/>
-      <c r="AC34" s="11"/>
-      <c r="AD34" s="11"/>
-      <c r="AE34" s="11"/>
-      <c r="AF34" s="11"/>
-      <c r="AG34" s="11"/>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A35" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="42">
-        <v>1</v>
-      </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="11"/>
-      <c r="AA35" s="11"/>
-      <c r="AB35" s="11"/>
-      <c r="AC35" s="11"/>
-      <c r="AD35" s="11"/>
-      <c r="AE35" s="11"/>
-      <c r="AF35" s="11"/>
-      <c r="AG35" s="11"/>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A36" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="42">
-        <v>1</v>
-      </c>
-      <c r="D36" s="49"/>
-      <c r="F36" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
-      <c r="AB36" s="11"/>
-      <c r="AC36" s="11"/>
-      <c r="AD36" s="11"/>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
-      <c r="AG36" s="11"/>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A37" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="B37" s="42">
-        <v>1</v>
-      </c>
-      <c r="D37" s="49"/>
-      <c r="G37" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="11"/>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="11"/>
-      <c r="AC37" s="11"/>
-      <c r="AD37" s="11"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
-      <c r="AG37" s="11"/>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A38" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="43">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>11</v>
-      </c>
-      <c r="D38" s="46"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="I38" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="J38" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="K38" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="L38" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="M38" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="N38" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
-      <c r="Q38" s="40"/>
-      <c r="R38" s="40"/>
-      <c r="S38" s="40"/>
-      <c r="T38" s="40"/>
-      <c r="U38" s="40"/>
-      <c r="V38" s="40"/>
-      <c r="W38" s="40"/>
-      <c r="X38" s="43"/>
-      <c r="Y38" s="11"/>
-      <c r="Z38" s="11"/>
-      <c r="AA38" s="11"/>
-      <c r="AB38" s="11"/>
-      <c r="AC38" s="11"/>
-      <c r="AD38" s="11"/>
-      <c r="AE38" s="11"/>
-      <c r="AF38" s="11"/>
-      <c r="AG38" s="11"/>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A39" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="B39" s="42">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>6</v>
-      </c>
-      <c r="D39" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X39" s="42"/>
-      <c r="Y39" s="11"/>
-      <c r="Z39" s="11"/>
-      <c r="AA39" s="11"/>
-      <c r="AB39" s="11"/>
-      <c r="AC39" s="11"/>
-      <c r="AD39" s="11"/>
-      <c r="AE39" s="11"/>
-      <c r="AF39" s="11"/>
-      <c r="AG39" s="11"/>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A40" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="43">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>140</v>
-      </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="F40" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="G40" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="H40" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="I40" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-      <c r="P40" s="40"/>
-      <c r="Q40" s="40"/>
-      <c r="R40" s="40"/>
-      <c r="S40" s="40"/>
-      <c r="T40" s="40"/>
-      <c r="U40" s="40"/>
-      <c r="V40" s="40"/>
-      <c r="W40" s="40"/>
-      <c r="X40" s="43"/>
-      <c r="Y40" s="11"/>
-      <c r="Z40" s="11"/>
-      <c r="AA40" s="11"/>
-      <c r="AB40" s="11"/>
-      <c r="AC40" s="11"/>
-      <c r="AD40" s="11"/>
-      <c r="AE40" s="11"/>
-      <c r="AF40" s="11"/>
-      <c r="AG40" s="11"/>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A41" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="B41" s="42">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X41" s="42"/>
-      <c r="Y41" s="11"/>
-      <c r="Z41" s="11"/>
-      <c r="AA41" s="11"/>
-      <c r="AB41" s="11"/>
-      <c r="AC41" s="11"/>
-      <c r="AD41" s="11"/>
-      <c r="AE41" s="11"/>
-      <c r="AF41" s="11"/>
-      <c r="AG41" s="11"/>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A42" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42" s="42">
-        <v>1</v>
-      </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X42" s="42"/>
-      <c r="Y42" s="11"/>
-      <c r="Z42" s="11"/>
-      <c r="AA42" s="11"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="11"/>
-      <c r="AD42" s="11"/>
-      <c r="AE42" s="11"/>
-      <c r="AF42" s="11"/>
-      <c r="AG42" s="11"/>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A43" s="42" t="s">
-        <v>139</v>
-      </c>
-      <c r="B43" s="42">
-        <v>1</v>
-      </c>
-      <c r="D43" s="49"/>
-      <c r="F43" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="J43" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="X43" s="42"/>
-      <c r="Y43" s="11"/>
-      <c r="Z43" s="11"/>
-      <c r="AA43" s="11"/>
-      <c r="AB43" s="11"/>
-      <c r="AC43" s="11"/>
-      <c r="AD43" s="11"/>
-      <c r="AE43" s="11"/>
-      <c r="AF43" s="11"/>
-      <c r="AG43" s="11"/>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A44" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B44" s="43">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>8</v>
-      </c>
-      <c r="D44" s="46"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="H44" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="I44" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="J44" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="K44" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40"/>
-      <c r="P44" s="40"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="40"/>
-      <c r="S44" s="40"/>
-      <c r="T44" s="40"/>
-      <c r="U44" s="40"/>
-      <c r="V44" s="40"/>
-      <c r="W44" s="40"/>
-      <c r="X44" s="43"/>
-      <c r="Y44" s="11"/>
-      <c r="Z44" s="11"/>
-      <c r="AA44" s="11"/>
-      <c r="AB44" s="11"/>
-      <c r="AC44" s="11"/>
-      <c r="AD44" s="11"/>
-      <c r="AE44" s="11"/>
-      <c r="AF44" s="11"/>
-      <c r="AG44" s="11"/>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="Y45" s="11"/>
-      <c r="Z45" s="11"/>
-      <c r="AA45" s="11"/>
-      <c r="AB45" s="11"/>
-      <c r="AC45" s="11"/>
-      <c r="AD45" s="11"/>
-      <c r="AE45" s="11"/>
-      <c r="AF45" s="11"/>
-      <c r="AG45" s="11"/>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="Y46" s="11"/>
-      <c r="Z46" s="11"/>
-      <c r="AA46" s="11"/>
-      <c r="AB46" s="11"/>
-      <c r="AC46" s="11"/>
-      <c r="AD46" s="11"/>
-      <c r="AE46" s="11"/>
-      <c r="AF46" s="11"/>
-      <c r="AG46" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A04060-45CA-49C0-9E02-FCC68C03B3FB}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11026,9 +11245,7 @@
       <c r="B8" s="45">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
-        <v>11</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="46"/>
       <c r="E8" s="40"/>
       <c r="F8" s="40"/>
@@ -11209,7 +11426,9 @@
       <c r="I13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="11"/>
+      <c r="J13" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="K13" t="s">
         <v>46</v>
       </c>
@@ -11238,6 +11457,9 @@
         <v>44</v>
       </c>
       <c r="J14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" t="s">
         <v>45</v>
       </c>
       <c r="L14" t="s">
@@ -11247,7 +11469,7 @@
         <v>147</v>
       </c>
       <c r="N14" t="s">
-        <v>46</v>
+        <v>146</v>
       </c>
       <c r="AQ14" s="42"/>
     </row>
@@ -11264,10 +11486,11 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="J15" s="11" t="s">
-        <v>44</v>
-      </c>
+      <c r="J15" s="11"/>
       <c r="K15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" t="s">
         <v>45</v>
       </c>
       <c r="M15" t="s">
@@ -11297,10 +11520,19 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="K16" t="s">
-        <v>44</v>
-      </c>
       <c r="L16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P16" t="s">
         <v>45</v>
       </c>
       <c r="Q16" t="s">
@@ -11330,10 +11562,28 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="L17" t="s">
-        <v>44</v>
-      </c>
       <c r="M17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R17" t="s">
+        <v>45</v>
+      </c>
+      <c r="S17" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" t="s">
         <v>45</v>
       </c>
       <c r="U17" t="s">
@@ -11360,10 +11610,19 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="M18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="Q18" t="s">
+        <v>44</v>
+      </c>
+      <c r="R18" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" t="s">
+        <v>44</v>
+      </c>
+      <c r="T18" t="s">
+        <v>44</v>
+      </c>
+      <c r="U18" t="s">
         <v>45</v>
       </c>
       <c r="V18" t="s">
@@ -11390,10 +11649,16 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="N19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="U19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W19" t="s">
+        <v>45</v>
+      </c>
+      <c r="X19" t="s">
         <v>45</v>
       </c>
       <c r="Y19" t="s">
@@ -11420,10 +11685,16 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="O20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P20" t="s">
+      <c r="V20" t="s">
+        <v>44</v>
+      </c>
+      <c r="W20" t="s">
+        <v>44</v>
+      </c>
+      <c r="X20" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y20" t="s">
         <v>45</v>
       </c>
       <c r="Z20" t="s">
@@ -11450,10 +11721,10 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="P21" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q21" t="s">
+      <c r="Y21" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z21" t="s">
         <v>45</v>
       </c>
       <c r="AA21" t="s">
@@ -11480,10 +11751,10 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="Q22" t="s">
-        <v>44</v>
-      </c>
-      <c r="R22" t="s">
+      <c r="Z22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA22" t="s">
         <v>45</v>
       </c>
       <c r="AB22" t="s">
@@ -11510,10 +11781,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="R23" t="s">
-        <v>44</v>
-      </c>
-      <c r="S23" t="s">
+      <c r="AA23" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB23" t="s">
         <v>45</v>
       </c>
       <c r="AC23" t="s">
@@ -11540,10 +11811,10 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="S24" t="s">
-        <v>44</v>
-      </c>
-      <c r="T24" t="s">
+      <c r="AB24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC24" t="s">
         <v>45</v>
       </c>
       <c r="AD24" t="s">
@@ -11570,10 +11841,10 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="T25" t="s">
-        <v>44</v>
-      </c>
-      <c r="U25" t="s">
+      <c r="AC25" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD25" t="s">
         <v>45</v>
       </c>
       <c r="AE25" t="s">
@@ -11600,10 +11871,10 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="U26" t="s">
-        <v>44</v>
-      </c>
-      <c r="V26" t="s">
+      <c r="AD26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE26" t="s">
         <v>45</v>
       </c>
       <c r="AF26" t="s">
@@ -11630,10 +11901,10 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="V27" t="s">
-        <v>44</v>
-      </c>
-      <c r="W27" t="s">
+      <c r="AE27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF27" t="s">
         <v>45</v>
       </c>
       <c r="AG27" t="s">
@@ -11660,10 +11931,10 @@
       <c r="F28" s="11"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="W28" t="s">
-        <v>44</v>
-      </c>
-      <c r="X28" t="s">
+      <c r="AF28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG28" t="s">
         <v>45</v>
       </c>
       <c r="AH28" t="s">
@@ -11690,10 +11961,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-      <c r="X29" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y29" t="s">
+      <c r="AG29" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH29" t="s">
         <v>45</v>
       </c>
       <c r="AI29" t="s">
@@ -11723,10 +11994,13 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="Y30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z30" t="s">
+      <c r="AH30" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI30" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ30" t="s">
         <v>45</v>
       </c>
       <c r="AK30" t="s">
@@ -11753,10 +12027,13 @@
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
-      <c r="Z31" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA31" t="s">
+      <c r="AI31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK31" t="s">
         <v>45</v>
       </c>
       <c r="AL31" t="s">
@@ -11777,9 +12054,7 @@
       <c r="B32" s="45">
         <v>3</v>
       </c>
-      <c r="C32" s="1">
-        <v>40</v>
-      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="46"/>
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
@@ -11803,12 +12078,8 @@
       <c r="X32" s="40"/>
       <c r="Y32" s="40"/>
       <c r="Z32" s="40"/>
-      <c r="AA32" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB32" s="40" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA32" s="40"/>
+      <c r="AB32" s="40"/>
       <c r="AC32" s="40"/>
       <c r="AD32" s="40"/>
       <c r="AE32" s="40"/>
@@ -11817,8 +12088,12 @@
       <c r="AH32" s="40"/>
       <c r="AI32" s="40"/>
       <c r="AJ32" s="40"/>
-      <c r="AK32" s="40"/>
-      <c r="AL32" s="40"/>
+      <c r="AK32" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL32" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="AM32" s="40" t="s">
         <v>46</v>
       </c>
@@ -11997,9 +12272,7 @@
       <c r="B39" s="45">
         <v>2</v>
       </c>
-      <c r="C39" s="1">
-        <v>11</v>
-      </c>
+      <c r="C39" s="1"/>
       <c r="D39" s="46"/>
       <c r="E39" s="40"/>
       <c r="F39" s="40"/>
@@ -12016,12 +12289,14 @@
         <v>46</v>
       </c>
       <c r="M39" s="40" t="s">
-        <v>147</v>
+        <v>46</v>
       </c>
       <c r="N39" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="O39" s="40"/>
+        <v>147</v>
+      </c>
+      <c r="O39" s="40" t="s">
+        <v>146</v>
+      </c>
       <c r="P39" s="40"/>
       <c r="Q39" s="40"/>
       <c r="R39" s="40"/>
@@ -12109,9 +12384,6 @@
       </c>
       <c r="B42" s="45">
         <v>3</v>
-      </c>
-      <c r="C42">
-        <v>9</v>
       </c>
       <c r="D42" s="46"/>
       <c r="E42" s="40"/>

</xml_diff>

<commit_message>
File structure changes and clean up for project submission
</commit_message>
<xml_diff>
--- a/performance/performance.xlsx
+++ b/performance/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Kitzan\Documents\GitHub\seng440-huffman-coding\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014AEC62-1710-4CC8-B0B5-27ED8D5CF524}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785D2504-AFB8-49F4-9C49-11CCE96C5CE3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="168">
   <si>
     <t>Percentage</t>
   </si>
@@ -496,19 +496,52 @@
     <t>257(n)+11</t>
   </si>
   <si>
-    <t>184(n)+28</t>
-  </si>
-  <si>
     <t>34(n)+30</t>
   </si>
   <si>
-    <t>Run Time</t>
-  </si>
-  <si>
     <t>n = char</t>
   </si>
   <si>
     <t>n = uint32</t>
+  </si>
+  <si>
+    <t>Total Cycles</t>
+  </si>
+  <si>
+    <t>Encode Cycles</t>
+  </si>
+  <si>
+    <t>Decode Cycles</t>
+  </si>
+  <si>
+    <t>Syscalls Cycles</t>
+  </si>
+  <si>
+    <t>204(n)+18</t>
+  </si>
+  <si>
+    <t>Simplified</t>
+  </si>
+  <si>
+    <t>Start up</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>Wrap up</t>
+  </si>
+  <si>
+    <t>49(n*5) + 12(n)</t>
+  </si>
+  <si>
+    <t>39(n*5) + 9(n)</t>
+  </si>
+  <si>
+    <t>27(n)</t>
+  </si>
+  <si>
+    <t>32(n) + 12(n/5)</t>
   </si>
 </sst>
 </file>
@@ -791,7 +824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -895,48 +928,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -964,9 +955,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -974,6 +962,57 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5167,13 +5206,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:rowOff>7936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>6349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5200,16 +5239,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>7936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>6349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5236,16 +5275,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>11112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5273,15 +5312,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:rowOff>7936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>603249</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>39687</xdr:rowOff>
+      <xdr:rowOff>184149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5609,7 +5648,7 @@
   <dimension ref="A2:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C21" sqref="C21:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5644,13 +5683,13 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D3" s="77">
         <v>8031625000</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -5665,9 +5704,9 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="58"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="20" t="s">
         <v>10</v>
       </c>
@@ -5680,9 +5719,9 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="65"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="73"/>
       <c r="E5" s="23" t="s">
         <v>13</v>
       </c>
@@ -5696,11 +5735,11 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="61"/>
-      <c r="C6" s="60" t="s">
+      <c r="B6" s="75"/>
+      <c r="C6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="57">
+      <c r="D6" s="71">
         <v>10975812500</v>
       </c>
       <c r="E6" s="20" t="s">
@@ -5715,9 +5754,9 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="58"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="20" t="s">
         <v>10</v>
       </c>
@@ -5730,9 +5769,9 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="61"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="65"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="23" t="s">
         <v>13</v>
       </c>
@@ -5746,11 +5785,11 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="61"/>
-      <c r="C9" s="60" t="s">
+      <c r="B9" s="75"/>
+      <c r="C9" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="57">
+      <c r="D9" s="71">
         <v>15213125000</v>
       </c>
       <c r="E9" s="26" t="s">
@@ -5765,9 +5804,9 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="20" t="s">
         <v>10</v>
       </c>
@@ -5780,9 +5819,9 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="59"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="28" t="s">
         <v>13</v>
       </c>
@@ -5800,13 +5839,13 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="64">
+      <c r="D12" s="77">
         <v>6658937500</v>
       </c>
       <c r="E12" s="20" t="s">
@@ -5825,9 +5864,9 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="58"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="20" t="s">
         <v>10</v>
       </c>
@@ -5844,9 +5883,9 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="65"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="23" t="s">
         <v>13</v>
       </c>
@@ -5864,11 +5903,11 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="61"/>
-      <c r="C15" s="60" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="57">
+      <c r="D15" s="71">
         <v>7234250000</v>
       </c>
       <c r="E15" s="20" t="s">
@@ -5887,9 +5926,9 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="58"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="20" t="s">
         <v>10</v>
       </c>
@@ -5906,9 +5945,9 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="65"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="23" t="s">
         <v>13</v>
       </c>
@@ -5926,11 +5965,11 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="61"/>
-      <c r="C18" s="60" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="57">
+      <c r="D18" s="71">
         <v>11646625000</v>
       </c>
       <c r="E18" s="20" t="s">
@@ -5949,9 +5988,9 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="58"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="20" t="s">
         <v>10</v>
       </c>
@@ -5968,9 +6007,9 @@
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="59"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="28" t="s">
         <v>13</v>
       </c>
@@ -5984,30 +6023,30 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D21" s="77">
         <v>6294375000</v>
       </c>
-      <c r="E21" s="77" t="s">
+      <c r="E21" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="78">
+      <c r="F21" s="64">
         <v>0.14197499999999999</v>
       </c>
-      <c r="G21" s="79">
+      <c r="G21" s="65">
         <f>_xlfn.CEILING.MATH(D21*F21)</f>
         <v>893643891</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="58"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="20" t="s">
         <v>10</v>
       </c>
@@ -6020,9 +6059,9 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="65"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="23" t="s">
         <v>13</v>
       </c>
@@ -6036,11 +6075,11 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="61"/>
-      <c r="C24" s="60" t="s">
+      <c r="B24" s="75"/>
+      <c r="C24" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="57">
+      <c r="D24" s="71">
         <v>6577687500</v>
       </c>
       <c r="E24" s="20" t="s">
@@ -6055,9 +6094,9 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="58"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="72"/>
       <c r="E25" s="20" t="s">
         <v>10</v>
       </c>
@@ -6070,9 +6109,9 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="65"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="23" t="s">
         <v>13</v>
       </c>
@@ -6086,11 +6125,11 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="61"/>
-      <c r="C27" s="60" t="s">
+      <c r="B27" s="75"/>
+      <c r="C27" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="57">
+      <c r="D27" s="71">
         <v>7765437500</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -6105,9 +6144,9 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="58"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="20" t="s">
         <v>10</v>
       </c>
@@ -6120,9 +6159,9 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="65"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="23" t="s">
         <v>13</v>
       </c>
@@ -6137,92 +6176,92 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="71"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="74"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="74"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="60"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="73"/>
-      <c r="G33" s="74"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="74"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="60"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="74"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="71"/>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="74"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="74"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="60"/>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="71"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="73"/>
-      <c r="G38" s="74"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="60"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -6279,7 +6318,7 @@
   <dimension ref="A2:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D15:D16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6317,8 +6356,8 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
-      <c r="B3" s="67" t="s">
-        <v>14</v>
+      <c r="B3" s="81" t="s">
+        <v>155</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>11</v>
@@ -6341,7 +6380,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
-      <c r="B4" s="68"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
@@ -6362,7 +6401,7 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="68"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="32" t="s">
         <v>12</v>
       </c>
@@ -6382,8 +6421,8 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="67" t="s">
-        <v>9</v>
+      <c r="B6" s="81" t="s">
+        <v>156</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>11</v>
@@ -6404,7 +6443,7 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="68"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -6424,7 +6463,7 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="68"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="32" t="s">
         <v>12</v>
       </c>
@@ -6444,8 +6483,8 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="67" t="s">
-        <v>10</v>
+      <c r="B9" s="81" t="s">
+        <v>157</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>11</v>
@@ -6466,7 +6505,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="68"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="16" t="s">
         <v>7</v>
       </c>
@@ -6486,7 +6525,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="68"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="32" t="s">
         <v>12</v>
       </c>
@@ -6506,8 +6545,8 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="67" t="s">
-        <v>13</v>
+      <c r="B12" s="81" t="s">
+        <v>158</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>11</v>
@@ -6528,7 +6567,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="68"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="16" t="s">
         <v>7</v>
       </c>
@@ -6548,19 +6587,19 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="80"/>
-      <c r="C14" s="81" t="s">
+      <c r="B14" s="83"/>
+      <c r="C14" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="67">
         <f>Performance!G23</f>
         <v>3454227113</v>
       </c>
-      <c r="E14" s="82">
+      <c r="E14" s="67">
         <f>Performance!G26</f>
         <v>3530080440</v>
       </c>
-      <c r="F14" s="83">
+      <c r="F14" s="68">
         <f>Performance!G29</f>
         <v>4582772941</v>
       </c>
@@ -6730,35 +6769,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894D5C8D-F7D4-420C-ADAD-D25C20CEEE3B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BC710D-19AA-4D12-98C6-2B8F098B36A0}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
-    <col min="3" max="3" width="7.90625" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.08984375" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="54" t="s">
         <v>8</v>
       </c>
@@ -6766,71 +6809,116 @@
         <v>6</v>
       </c>
       <c r="D2" s="54" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="55" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" s="55" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="45" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="45">
+        <v>22</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="45">
+        <v>8</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="H3" s="84">
+        <v>0.2059</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="56" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" s="69">
-        <v>0.2059</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="56" t="s">
-        <v>155</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="42">
+        <v>17</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" s="42">
+        <v>6</v>
+      </c>
+      <c r="G4" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="70"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H4" s="85"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="45" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="45">
+        <v>11</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="45">
+        <v>0</v>
+      </c>
+      <c r="G5" s="70" t="s">
         <v>151</v>
       </c>
-      <c r="E5" s="69">
-        <v>0.28399999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H5" s="84">
+        <v>0.20599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="56" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="D6" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="70"/>
+      <c r="D6" s="42">
+        <v>13</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="42">
+        <v>5</v>
+      </c>
+      <c r="G6" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6839,7 +6927,7 @@
   <dimension ref="A1:BK28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="AD26" sqref="AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7830,13 +7918,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F74B2D-652B-4E3A-A8D3-572CE0B18B69}">
   <dimension ref="A1:AG46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="26.08984375" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" customWidth="1"/>
     <col min="4" max="33" width="2.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9602,10 +9691,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E3818A-D03F-4D14-9726-3113DF885761}">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9613,11 +9702,11 @@
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="6.81640625" customWidth="1"/>
     <col min="3" max="3" width="6.26953125" customWidth="1"/>
-    <col min="4" max="27" width="2.7265625" customWidth="1"/>
-    <col min="28" max="31" width="10.90625" customWidth="1"/>
+    <col min="4" max="31" width="2.7265625" customWidth="1"/>
+    <col min="32" max="35" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>41</v>
       </c>
@@ -9694,16 +9783,28 @@
       <c r="Z1" s="49">
         <v>23</v>
       </c>
-      <c r="AA1" s="47">
+      <c r="AA1" s="49">
         <v>24</v>
       </c>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="1"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AB1" s="49">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="49">
+        <v>26</v>
+      </c>
+      <c r="AD1" s="49">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="47">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="1"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
         <v>46</v>
       </c>
@@ -9725,14 +9826,14 @@
       <c r="H2" t="s">
         <v>145</v>
       </c>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
+      <c r="AE2" s="38"/>
       <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
         <v>47</v>
       </c>
@@ -9755,14 +9856,14 @@
       <c r="I3" t="s">
         <v>145</v>
       </c>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
+      <c r="AE3" s="38"/>
       <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
         <v>48</v>
       </c>
@@ -9785,14 +9886,14 @@
       <c r="J4" t="s">
         <v>145</v>
       </c>
-      <c r="AA4" s="38"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
+      <c r="AE4" s="38"/>
       <c r="AF4" s="1"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
         <v>49</v>
       </c>
@@ -9815,14 +9916,14 @@
       <c r="K5" t="s">
         <v>145</v>
       </c>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
+      <c r="AE5" s="38"/>
       <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
         <v>50</v>
       </c>
@@ -9845,14 +9946,14 @@
       <c r="L6" t="s">
         <v>145</v>
       </c>
-      <c r="AA6" s="38"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
+      <c r="AE6" s="38"/>
       <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
         <v>51</v>
       </c>
@@ -9875,14 +9976,14 @@
       <c r="M7" t="s">
         <v>145</v>
       </c>
-      <c r="AA7" s="38"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
+      <c r="AE7" s="38"/>
       <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
         <v>52</v>
       </c>
@@ -9905,14 +10006,14 @@
       <c r="N8" t="s">
         <v>145</v>
       </c>
-      <c r="AA8" s="38"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
+      <c r="AE8" s="38"/>
       <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
         <v>53</v>
       </c>
@@ -9935,19 +10036,22 @@
       <c r="O9" t="s">
         <v>145</v>
       </c>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
+      <c r="AE9" s="38"/>
       <c r="AF9" s="1"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="41">
         <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="36"/>
@@ -9982,23 +10086,24 @@
       <c r="X10" s="36"/>
       <c r="Y10" s="36"/>
       <c r="Z10" s="36"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
+      <c r="AA10" s="36"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="36"/>
+      <c r="AD10" s="36"/>
+      <c r="AE10" s="39"/>
       <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="40">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>141</v>
-      </c>
       <c r="D11" s="45" t="s">
         <v>43</v>
       </c>
@@ -10014,14 +10119,14 @@
       <c r="H11" t="s">
         <v>145</v>
       </c>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
+      <c r="AE11" s="38"/>
       <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
         <v>61</v>
       </c>
@@ -10044,14 +10149,14 @@
       <c r="I12" t="s">
         <v>145</v>
       </c>
-      <c r="AA12" s="38"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
+      <c r="AE12" s="38"/>
       <c r="AF12" s="1"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
         <v>62</v>
       </c>
@@ -10074,14 +10179,14 @@
       <c r="J13" t="s">
         <v>145</v>
       </c>
-      <c r="AA13" s="38"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
+      <c r="AE13" s="38"/>
       <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="s">
         <v>63</v>
       </c>
@@ -10104,14 +10209,14 @@
       <c r="K14" t="s">
         <v>145</v>
       </c>
-      <c r="AA14" s="38"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
+      <c r="AE14" s="38"/>
       <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
         <v>64</v>
       </c>
@@ -10134,14 +10239,14 @@
       <c r="L15" t="s">
         <v>145</v>
       </c>
-      <c r="AA15" s="38"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
+      <c r="AE15" s="38"/>
       <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
         <v>65</v>
       </c>
@@ -10156,22 +10261,28 @@
         <v>44</v>
       </c>
       <c r="K16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L16" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="M16" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA16" s="38"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="N16" t="s">
+        <v>146</v>
+      </c>
+      <c r="O16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE16" s="38"/>
       <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="s">
         <v>66</v>
       </c>
@@ -10183,25 +10294,37 @@
         <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M17" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="N17" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="O17" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>146</v>
+      </c>
+      <c r="R17" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE17" s="38"/>
       <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
         <v>67</v>
       </c>
@@ -10209,29 +10332,35 @@
         <v>1</v>
       </c>
       <c r="D18" s="45"/>
-      <c r="K18" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" t="s">
-        <v>44</v>
-      </c>
       <c r="M18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N18" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="O18" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA18" s="38"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="P18" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>45</v>
+      </c>
+      <c r="R18" t="s">
+        <v>146</v>
+      </c>
+      <c r="S18" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE18" s="38"/>
       <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19" s="38" t="s">
         <v>68</v>
       </c>
@@ -10245,30 +10374,30 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="M19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE19" s="38"/>
       <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20" s="38" t="s">
         <v>69</v>
       </c>
@@ -10276,29 +10405,29 @@
         <v>1</v>
       </c>
       <c r="D20" s="45"/>
-      <c r="M20" t="s">
-        <v>43</v>
-      </c>
-      <c r="N20" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" t="s">
-        <v>146</v>
-      </c>
       <c r="Q20" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA20" s="38"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="R20" t="s">
+        <v>44</v>
+      </c>
+      <c r="S20" t="s">
+        <v>45</v>
+      </c>
+      <c r="T20" t="s">
+        <v>146</v>
+      </c>
+      <c r="U20" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE20" s="38"/>
       <c r="AF20" s="1"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A21" s="38" t="s">
         <v>70</v>
       </c>
@@ -10306,29 +10435,29 @@
         <v>1</v>
       </c>
       <c r="D21" s="45"/>
-      <c r="N21" t="s">
-        <v>43</v>
-      </c>
-      <c r="O21" t="s">
-        <v>44</v>
-      </c>
-      <c r="P21" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>146</v>
-      </c>
       <c r="R21" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA21" s="38"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="S21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T21" t="s">
+        <v>45</v>
+      </c>
+      <c r="U21" t="s">
+        <v>146</v>
+      </c>
+      <c r="V21" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE21" s="38"/>
       <c r="AF21" s="1"/>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A22" s="38" t="s">
         <v>71</v>
       </c>
@@ -10336,29 +10465,29 @@
         <v>1</v>
       </c>
       <c r="D22" s="45"/>
-      <c r="O22" t="s">
-        <v>43</v>
-      </c>
-      <c r="P22" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>45</v>
-      </c>
-      <c r="R22" t="s">
-        <v>146</v>
-      </c>
       <c r="S22" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA22" s="38"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="T22" t="s">
+        <v>44</v>
+      </c>
+      <c r="U22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V22" t="s">
+        <v>146</v>
+      </c>
+      <c r="W22" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE22" s="38"/>
       <c r="AF22" s="1"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" s="38" t="s">
         <v>72</v>
       </c>
@@ -10366,29 +10495,29 @@
         <v>1</v>
       </c>
       <c r="D23" s="45"/>
-      <c r="P23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>44</v>
-      </c>
-      <c r="R23" t="s">
-        <v>45</v>
-      </c>
-      <c r="S23" t="s">
-        <v>146</v>
-      </c>
       <c r="T23" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA23" s="38"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="U23" t="s">
+        <v>44</v>
+      </c>
+      <c r="V23" t="s">
+        <v>45</v>
+      </c>
+      <c r="W23" t="s">
+        <v>146</v>
+      </c>
+      <c r="X23" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE23" s="38"/>
       <c r="AF23" s="1"/>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" s="38" t="s">
         <v>73</v>
       </c>
@@ -10396,29 +10525,29 @@
         <v>1</v>
       </c>
       <c r="D24" s="45"/>
-      <c r="Q24" t="s">
-        <v>43</v>
-      </c>
-      <c r="R24" t="s">
-        <v>44</v>
-      </c>
-      <c r="S24" t="s">
-        <v>45</v>
-      </c>
-      <c r="T24" t="s">
-        <v>146</v>
-      </c>
       <c r="U24" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA24" s="38"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-      <c r="AE24" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="V24" t="s">
+        <v>44</v>
+      </c>
+      <c r="W24" t="s">
+        <v>45</v>
+      </c>
+      <c r="X24" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE24" s="38"/>
       <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
         <v>36</v>
       </c>
@@ -10426,29 +10555,29 @@
         <v>1</v>
       </c>
       <c r="D25" s="45"/>
-      <c r="R25" t="s">
-        <v>43</v>
-      </c>
-      <c r="S25" t="s">
-        <v>44</v>
-      </c>
-      <c r="T25" t="s">
-        <v>45</v>
-      </c>
-      <c r="U25" t="s">
-        <v>146</v>
-      </c>
       <c r="V25" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="W25" t="s">
+        <v>44</v>
+      </c>
+      <c r="X25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE25" s="38"/>
       <c r="AF25" s="1"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A26" s="38" t="s">
         <v>74</v>
       </c>
@@ -10456,32 +10585,32 @@
         <v>2</v>
       </c>
       <c r="D26" s="45"/>
-      <c r="S26" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="T26" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="U26" t="s">
-        <v>45</v>
-      </c>
-      <c r="V26" t="s">
-        <v>45</v>
-      </c>
-      <c r="W26" t="s">
-        <v>146</v>
-      </c>
-      <c r="X26" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA26" s="38"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="1"/>
+      <c r="W26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="X26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE26" s="38"/>
       <c r="AF26" s="1"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A27" s="39" t="s">
         <v>75</v>
       </c>
@@ -10504,37 +10633,41 @@
       <c r="Q27" s="36"/>
       <c r="R27" s="36"/>
       <c r="S27" s="36"/>
-      <c r="T27" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="U27" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="V27" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="W27" s="36" t="s">
-        <v>45</v>
-      </c>
+      <c r="T27" s="36"/>
+      <c r="U27" s="36"/>
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
       <c r="X27" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Y27" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z27" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA27" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="AA27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD27" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE27" s="39" t="s">
+        <v>145</v>
+      </c>
       <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A28" s="38" t="s">
         <v>76</v>
       </c>
@@ -10556,14 +10689,14 @@
       <c r="H28" t="s">
         <v>145</v>
       </c>
-      <c r="AA28" s="38"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
+      <c r="AE28" s="38"/>
       <c r="AF28" s="1"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A29" s="38" t="s">
         <v>49</v>
       </c>
@@ -10586,14 +10719,14 @@
       <c r="I29" t="s">
         <v>145</v>
       </c>
-      <c r="AA29" s="38"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
+      <c r="AE29" s="38"/>
       <c r="AF29" s="1"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A30" s="38" t="s">
         <v>55</v>
       </c>
@@ -10616,14 +10749,14 @@
       <c r="J30" t="s">
         <v>145</v>
       </c>
-      <c r="AA30" s="38"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
+      <c r="AE30" s="38"/>
       <c r="AF30" s="1"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG30" s="1"/>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A31" s="39" t="s">
         <v>56</v>
       </c>
@@ -10665,14 +10798,18 @@
       <c r="X31" s="36"/>
       <c r="Y31" s="36"/>
       <c r="Z31" s="36"/>
-      <c r="AA31" s="39"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="1"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AD31" s="36"/>
+      <c r="AE31" s="39"/>
       <c r="AF31" s="1"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG31" s="1"/>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A32" s="38" t="s">
         <v>57</v>
       </c>
@@ -10697,14 +10834,14 @@
       <c r="H32" t="s">
         <v>145</v>
       </c>
-      <c r="AA32" s="38"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AE32" s="1"/>
+      <c r="AE32" s="38"/>
       <c r="AF32" s="1"/>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
         <v>52</v>
       </c>
@@ -10727,14 +10864,14 @@
       <c r="I33" t="s">
         <v>145</v>
       </c>
-      <c r="AA33" s="38"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
+      <c r="AE33" s="38"/>
       <c r="AF33" s="1"/>
-    </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG33" s="1"/>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A34" s="38" t="s">
         <v>53</v>
       </c>
@@ -10757,14 +10894,14 @@
       <c r="J34" t="s">
         <v>145</v>
       </c>
-      <c r="AA34" s="38"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-      <c r="AE34" s="1"/>
+      <c r="AE34" s="38"/>
       <c r="AF34" s="1"/>
-    </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG34" s="1"/>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A35" s="38" t="s">
         <v>54</v>
       </c>
@@ -10787,14 +10924,14 @@
       <c r="K35" t="s">
         <v>145</v>
       </c>
-      <c r="AA35" s="38"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="1"/>
-      <c r="AE35" s="1"/>
+      <c r="AE35" s="38"/>
       <c r="AF35" s="1"/>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG35" s="1"/>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -10838,14 +10975,18 @@
       <c r="X36" s="36"/>
       <c r="Y36" s="36"/>
       <c r="Z36" s="36"/>
-      <c r="AA36" s="39"/>
-      <c r="AB36" s="1"/>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="1"/>
-      <c r="AE36" s="1"/>
+      <c r="AA36" s="36"/>
+      <c r="AB36" s="36"/>
+      <c r="AC36" s="36"/>
+      <c r="AD36" s="36"/>
+      <c r="AE36" s="39"/>
       <c r="AF36" s="1"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="AG36" s="1"/>
+      <c r="AH36" s="1"/>
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A37" s="43" t="s">
         <v>59</v>
       </c>
@@ -10885,15 +11026,20 @@
       <c r="X37" s="36"/>
       <c r="Y37" s="36"/>
       <c r="Z37" s="36"/>
-      <c r="AA37" s="39"/>
-      <c r="AB37" s="1"/>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
+      <c r="AA37" s="36"/>
+      <c r="AB37" s="36"/>
+      <c r="AC37" s="36"/>
+      <c r="AD37" s="36"/>
+      <c r="AE37" s="39"/>
       <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+      <c r="AH37" s="1"/>
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10901,14 +11047,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A04060-45CA-49C0-9E02-FCC68C03B3FB}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.90625" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" customWidth="1"/>
     <col min="3" max="3" width="6.1796875" customWidth="1"/>
     <col min="4" max="43" width="2.6328125" customWidth="1"/>
   </cols>
@@ -12405,5 +12551,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assembly fixes, report, and new perfromance statistics
</commit_message>
<xml_diff>
--- a/performance/performance.xlsx
+++ b/performance/performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Kitzan\Documents\GitHub\seng440-huffman-coding\performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E261A796-4E7F-46A2-AE08-4A4988D02F45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF4510B-AD87-459C-89A1-739F236FDEAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{75AA8218-EDBD-4373-90E6-0865F94C811F}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="Encode GCC" sheetId="7" r:id="rId6"/>
     <sheet name="Decode OPT" sheetId="5" r:id="rId7"/>
     <sheet name="Decode GCC" sheetId="6" r:id="rId8"/>
+    <sheet name="Decode UNIT" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="195">
   <si>
     <t>Percentage</t>
   </si>
@@ -481,18 +482,9 @@
     <t>GCC</t>
   </si>
   <si>
-    <t>27(n)+23</t>
-  </si>
-  <si>
     <t>Improvement</t>
   </si>
   <si>
-    <t>257(n)+11</t>
-  </si>
-  <si>
-    <t>34(n)+30</t>
-  </si>
-  <si>
     <t>n = char</t>
   </si>
   <si>
@@ -511,9 +503,6 @@
     <t>Syscalls Cycles</t>
   </si>
   <si>
-    <t>204(n)+18</t>
-  </si>
-  <si>
     <t>Simplified</t>
   </si>
   <si>
@@ -529,9 +518,6 @@
     <t>49(n*5) + 12(n)</t>
   </si>
   <si>
-    <t>39(n*5) + 9(n)</t>
-  </si>
-  <si>
     <t>27(n)</t>
   </si>
   <si>
@@ -545,6 +531,99 @@
   </si>
   <si>
     <t>Labels</t>
+  </si>
+  <si>
+    <t>mov   r8, r0</t>
+  </si>
+  <si>
+    <t>mov   r2, r1</t>
+  </si>
+  <si>
+    <t>ldr   r9, [r8, #4]!</t>
+  </si>
+  <si>
+    <t>ldr   r5, [r0]</t>
+  </si>
+  <si>
+    <t>mov   r4, #0</t>
+  </si>
+  <si>
+    <t>mov   r0, r5</t>
+  </si>
+  <si>
+    <t>bl    lookup_unit</t>
+  </si>
+  <si>
+    <t>ubfx  ip, r0, #8, #8</t>
+  </si>
+  <si>
+    <t>lsr   r3, r9, r4</t>
+  </si>
+  <si>
+    <t>rsb   r6, ip, #32</t>
+  </si>
+  <si>
+    <t>add   r4, r4, ip</t>
+  </si>
+  <si>
+    <t>uxtb  r7, r0</t>
+  </si>
+  <si>
+    <t>lsl   r3, r3, r6</t>
+  </si>
+  <si>
+    <t>tst   r4, #32</t>
+  </si>
+  <si>
+    <t>orr   r5, r3, r5, lsr ip</t>
+  </si>
+  <si>
+    <t>strb  r7, [r1], #1</t>
+  </si>
+  <si>
+    <t>beq   .L11</t>
+  </si>
+  <si>
+    <t>subs  r4, r4, #32</t>
+  </si>
+  <si>
+    <t>rsbne r3, r4, #32</t>
+  </si>
+  <si>
+    <t>orrne r5, r5, r9, lsl r3</t>
+  </si>
+  <si>
+    <t>cmp   r7, #3</t>
+  </si>
+  <si>
+    <t>bne   .L12</t>
+  </si>
+  <si>
+    <t>sub   r0, r1, r2</t>
+  </si>
+  <si>
+    <t>UNIT</t>
+  </si>
+  <si>
+    <t>27(n*5) + 11(n)</t>
+  </si>
+  <si>
+    <t>39(n*5) + 11(n)</t>
+  </si>
+  <si>
+    <t>146(n) + 18</t>
+  </si>
+  <si>
+    <t>206(n) + 18</t>
+  </si>
+  <si>
+    <t>34(n) + 30</t>
+  </si>
+  <si>
+    <t>27(n) + 23</t>
+  </si>
+  <si>
+    <t>257(n) + 11</t>
   </si>
 </sst>
 </file>
@@ -613,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -833,12 +912,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -977,21 +1067,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -1001,11 +1081,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1022,11 +1117,18 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5697,13 +5799,13 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="77">
         <v>8031625000</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -5718,8 +5820,8 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
       <c r="D4" s="72"/>
       <c r="E4" s="20" t="s">
         <v>10</v>
@@ -5733,8 +5835,8 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="67"/>
-      <c r="C5" s="68"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="73"/>
       <c r="E5" s="23" t="s">
         <v>13</v>
@@ -5749,8 +5851,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="67"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="75"/>
+      <c r="C6" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="71">
@@ -5768,8 +5870,8 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="72"/>
       <c r="E7" s="20" t="s">
         <v>10</v>
@@ -5783,8 +5885,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="76"/>
       <c r="D8" s="73"/>
       <c r="E8" s="23" t="s">
         <v>13</v>
@@ -5799,8 +5901,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="67"/>
-      <c r="C9" s="69" t="s">
+      <c r="B9" s="75"/>
+      <c r="C9" s="74" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="71">
@@ -5818,8 +5920,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
       <c r="D10" s="72"/>
       <c r="E10" s="20" t="s">
         <v>10</v>
@@ -5833,9 +5935,9 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="70"/>
-      <c r="C11" s="70"/>
-      <c r="D11" s="75"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="28" t="s">
         <v>13</v>
       </c>
@@ -5853,13 +5955,13 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="74">
+      <c r="D12" s="77">
         <v>6658937500</v>
       </c>
       <c r="E12" s="20" t="s">
@@ -5878,8 +5980,8 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
       <c r="D13" s="72"/>
       <c r="E13" s="20" t="s">
         <v>10</v>
@@ -5897,8 +5999,8 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="73"/>
       <c r="E14" s="23" t="s">
         <v>13</v>
@@ -5917,8 +6019,8 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="67"/>
-      <c r="C15" s="69" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="71">
@@ -5940,8 +6042,8 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="72"/>
       <c r="E16" s="20" t="s">
         <v>10</v>
@@ -5959,8 +6061,8 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="67"/>
-      <c r="C17" s="68"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="73"/>
       <c r="E17" s="23" t="s">
         <v>13</v>
@@ -5979,8 +6081,8 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="67"/>
-      <c r="C18" s="69" t="s">
+      <c r="B18" s="75"/>
+      <c r="C18" s="74" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="71">
@@ -6002,8 +6104,8 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="72"/>
       <c r="E19" s="20" t="s">
         <v>10</v>
@@ -6021,9 +6123,9 @@
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="75"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="28" t="s">
         <v>13</v>
       </c>
@@ -6037,13 +6139,13 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="74">
+      <c r="D21" s="77">
         <v>6294375000</v>
       </c>
       <c r="E21" s="58" t="s">
@@ -6058,8 +6160,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
       <c r="D22" s="72"/>
       <c r="E22" s="20" t="s">
         <v>10</v>
@@ -6073,8 +6175,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="67"/>
-      <c r="C23" s="68"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="73"/>
       <c r="E23" s="23" t="s">
         <v>13</v>
@@ -6089,8 +6191,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="67"/>
-      <c r="C24" s="69" t="s">
+      <c r="B24" s="75"/>
+      <c r="C24" s="74" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="71">
@@ -6108,8 +6210,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="72"/>
       <c r="E25" s="20" t="s">
         <v>10</v>
@@ -6123,8 +6225,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="67"/>
-      <c r="C26" s="68"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="73"/>
       <c r="E26" s="23" t="s">
         <v>13</v>
@@ -6139,8 +6241,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="67"/>
-      <c r="C27" s="69" t="s">
+      <c r="B27" s="75"/>
+      <c r="C27" s="74" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="71">
@@ -6158,8 +6260,8 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
       <c r="D28" s="72"/>
       <c r="E28" s="20" t="s">
         <v>10</v>
@@ -6173,8 +6275,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
       <c r="D29" s="73"/>
       <c r="E29" s="23" t="s">
         <v>13</v>
@@ -6300,6 +6402,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B21:B29"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B20"/>
     <mergeCell ref="D27:D29"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C27:C29"/>
@@ -6311,16 +6423,6 @@
     <mergeCell ref="D18:D20"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="D24:D26"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6370,8 +6472,8 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
-      <c r="B3" s="76" t="s">
-        <v>153</v>
+      <c r="B3" s="81" t="s">
+        <v>150</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>11</v>
@@ -6394,7 +6496,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
-      <c r="B4" s="77"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
@@ -6415,7 +6517,7 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="77"/>
+      <c r="B5" s="82"/>
       <c r="C5" s="32" t="s">
         <v>12</v>
       </c>
@@ -6435,8 +6537,8 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="76" t="s">
-        <v>154</v>
+      <c r="B6" s="81" t="s">
+        <v>151</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>11</v>
@@ -6457,7 +6559,7 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="77"/>
+      <c r="B7" s="82"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
@@ -6477,7 +6579,7 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="77"/>
+      <c r="B8" s="82"/>
       <c r="C8" s="32" t="s">
         <v>12</v>
       </c>
@@ -6497,8 +6599,8 @@
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="76" t="s">
-        <v>155</v>
+      <c r="B9" s="81" t="s">
+        <v>152</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>11</v>
@@ -6519,7 +6621,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="77"/>
+      <c r="B10" s="82"/>
       <c r="C10" s="16" t="s">
         <v>7</v>
       </c>
@@ -6539,7 +6641,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="77"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="32" t="s">
         <v>12</v>
       </c>
@@ -6559,8 +6661,8 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="76" t="s">
-        <v>156</v>
+      <c r="B12" s="81" t="s">
+        <v>153</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>11</v>
@@ -6581,7 +6683,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="77"/>
+      <c r="B13" s="82"/>
       <c r="C13" s="16" t="s">
         <v>7</v>
       </c>
@@ -6601,7 +6703,7 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="78"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="61" t="s">
         <v>12</v>
       </c>
@@ -6797,10 +6899,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BC710D-19AA-4D12-98C6-2B8F098B36A0}">
-  <dimension ref="B2:H6"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6809,9 +6911,9 @@
     <col min="2" max="2" width="9.7265625" customWidth="1"/>
     <col min="3" max="3" width="8.08984375" customWidth="1"/>
     <col min="4" max="4" width="8.26953125" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" customWidth="1"/>
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6823,19 +6925,19 @@
         <v>6</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F2" s="49" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
@@ -6849,21 +6951,21 @@
         <v>22</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F3" s="44">
         <v>8</v>
       </c>
       <c r="G3" s="65" t="s">
-        <v>150</v>
-      </c>
-      <c r="H3" s="79">
+        <v>192</v>
+      </c>
+      <c r="H3" s="84">
         <v>0.2059</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>145</v>
@@ -6872,15 +6974,15 @@
         <v>17</v>
       </c>
       <c r="E4" s="64" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F4" s="42">
         <v>6</v>
       </c>
       <c r="G4" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="80"/>
+        <v>193</v>
+      </c>
+      <c r="H4" s="85"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="44" t="s">
@@ -6893,21 +6995,21 @@
         <v>11</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F5" s="44">
         <v>0</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="79">
-        <v>0.20599999999999999</v>
+        <v>194</v>
+      </c>
+      <c r="H5" s="84">
+        <v>0.19839999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="51" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>145</v>
@@ -6916,20 +7018,88 @@
         <v>13</v>
       </c>
       <c r="E6" s="64" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="F6" s="42">
         <v>5</v>
       </c>
       <c r="G6" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="H6" s="85"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="H6" s="80"/>
+      <c r="G10" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="87">
+        <v>13</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" s="87">
+        <v>5</v>
+      </c>
+      <c r="G11" s="89" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" s="84">
+        <v>0.2913</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="41">
+        <v>10</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" s="41">
+        <v>5</v>
+      </c>
+      <c r="G12" s="91" t="s">
+        <v>190</v>
+      </c>
+      <c r="H12" s="85"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H11:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6958,94 +7128,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:63" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="84" t="s">
+      <c r="A1" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="82">
-        <v>1</v>
-      </c>
-      <c r="E1" s="82">
+      <c r="C1" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="67">
+        <v>1</v>
+      </c>
+      <c r="E1" s="67">
         <v>2</v>
       </c>
-      <c r="F1" s="82">
+      <c r="F1" s="67">
         <v>3</v>
       </c>
-      <c r="G1" s="82">
+      <c r="G1" s="67">
         <v>4</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="67">
         <v>5</v>
       </c>
-      <c r="I1" s="82">
+      <c r="I1" s="67">
         <v>6</v>
       </c>
-      <c r="J1" s="82">
+      <c r="J1" s="67">
         <v>7</v>
       </c>
-      <c r="K1" s="82">
+      <c r="K1" s="67">
         <v>8</v>
       </c>
-      <c r="L1" s="82">
+      <c r="L1" s="67">
         <v>9</v>
       </c>
-      <c r="M1" s="82">
+      <c r="M1" s="67">
         <v>10</v>
       </c>
-      <c r="N1" s="82">
+      <c r="N1" s="67">
         <v>11</v>
       </c>
-      <c r="O1" s="82">
+      <c r="O1" s="67">
         <v>12</v>
       </c>
-      <c r="P1" s="82">
+      <c r="P1" s="67">
         <v>13</v>
       </c>
-      <c r="Q1" s="82">
+      <c r="Q1" s="67">
         <v>14</v>
       </c>
-      <c r="R1" s="82">
+      <c r="R1" s="67">
         <v>15</v>
       </c>
-      <c r="S1" s="82">
+      <c r="S1" s="67">
         <v>16</v>
       </c>
-      <c r="T1" s="82">
+      <c r="T1" s="67">
         <v>17</v>
       </c>
-      <c r="U1" s="82">
+      <c r="U1" s="67">
         <v>18</v>
       </c>
-      <c r="V1" s="82">
+      <c r="V1" s="67">
         <v>19</v>
       </c>
-      <c r="W1" s="82">
+      <c r="W1" s="67">
         <v>20</v>
       </c>
-      <c r="X1" s="82">
+      <c r="X1" s="67">
         <v>21</v>
       </c>
-      <c r="Y1" s="82">
+      <c r="Y1" s="67">
         <v>22</v>
       </c>
-      <c r="Z1" s="82">
+      <c r="Z1" s="67">
         <v>23</v>
       </c>
-      <c r="AA1" s="82">
+      <c r="AA1" s="67">
         <v>24</v>
       </c>
-      <c r="AB1" s="82">
+      <c r="AB1" s="67">
         <v>25</v>
       </c>
-      <c r="AC1" s="82">
+      <c r="AC1" s="67">
         <v>26</v>
       </c>
-      <c r="AD1" s="83">
+      <c r="AD1" s="68">
         <v>27</v>
       </c>
       <c r="AE1" s="45"/>
@@ -7948,76 +8118,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="83" t="s">
+      <c r="A1" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="81">
-        <v>1</v>
-      </c>
-      <c r="E1" s="82">
+      <c r="C1" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="66">
+        <v>1</v>
+      </c>
+      <c r="E1" s="67">
         <v>2</v>
       </c>
-      <c r="F1" s="82">
+      <c r="F1" s="67">
         <v>3</v>
       </c>
-      <c r="G1" s="82">
+      <c r="G1" s="67">
         <v>4</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="67">
         <v>5</v>
       </c>
-      <c r="I1" s="82">
+      <c r="I1" s="67">
         <v>6</v>
       </c>
-      <c r="J1" s="82">
+      <c r="J1" s="67">
         <v>7</v>
       </c>
-      <c r="K1" s="82">
+      <c r="K1" s="67">
         <v>8</v>
       </c>
-      <c r="L1" s="82">
+      <c r="L1" s="67">
         <v>9</v>
       </c>
-      <c r="M1" s="82">
+      <c r="M1" s="67">
         <v>10</v>
       </c>
-      <c r="N1" s="82">
+      <c r="N1" s="67">
         <v>11</v>
       </c>
-      <c r="O1" s="82">
+      <c r="O1" s="67">
         <v>12</v>
       </c>
-      <c r="P1" s="82">
+      <c r="P1" s="67">
         <v>13</v>
       </c>
-      <c r="Q1" s="82">
+      <c r="Q1" s="67">
         <v>14</v>
       </c>
-      <c r="R1" s="82">
+      <c r="R1" s="67">
         <v>15</v>
       </c>
-      <c r="S1" s="82">
+      <c r="S1" s="67">
         <v>16</v>
       </c>
-      <c r="T1" s="82">
+      <c r="T1" s="67">
         <v>17</v>
       </c>
-      <c r="U1" s="82">
+      <c r="U1" s="67">
         <v>18</v>
       </c>
-      <c r="V1" s="82">
+      <c r="V1" s="67">
         <v>19</v>
       </c>
-      <c r="W1" s="82">
+      <c r="W1" s="67">
         <v>20</v>
       </c>
-      <c r="X1" s="83">
+      <c r="X1" s="68">
         <v>21</v>
       </c>
       <c r="Y1" s="46"/>
@@ -9723,8 +9893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E3818A-D03F-4D14-9726-3113DF885761}">
   <dimension ref="A1:AJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9737,97 +9907,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="84" t="s">
+      <c r="A1" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="84" t="s">
-        <v>168</v>
-      </c>
-      <c r="D1" s="81">
-        <v>1</v>
-      </c>
-      <c r="E1" s="82">
+      <c r="C1" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="66">
+        <v>1</v>
+      </c>
+      <c r="E1" s="67">
         <v>2</v>
       </c>
-      <c r="F1" s="82">
+      <c r="F1" s="67">
         <v>3</v>
       </c>
-      <c r="G1" s="82">
+      <c r="G1" s="67">
         <v>4</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="67">
         <v>5</v>
       </c>
-      <c r="I1" s="82">
+      <c r="I1" s="67">
         <v>6</v>
       </c>
-      <c r="J1" s="82">
+      <c r="J1" s="67">
         <v>7</v>
       </c>
-      <c r="K1" s="82">
+      <c r="K1" s="67">
         <v>8</v>
       </c>
-      <c r="L1" s="82">
+      <c r="L1" s="67">
         <v>9</v>
       </c>
-      <c r="M1" s="82">
+      <c r="M1" s="67">
         <v>10</v>
       </c>
-      <c r="N1" s="82">
+      <c r="N1" s="67">
         <v>11</v>
       </c>
-      <c r="O1" s="82">
+      <c r="O1" s="67">
         <v>12</v>
       </c>
-      <c r="P1" s="82">
+      <c r="P1" s="67">
         <v>13</v>
       </c>
-      <c r="Q1" s="82">
+      <c r="Q1" s="67">
         <v>14</v>
       </c>
-      <c r="R1" s="82">
+      <c r="R1" s="67">
         <v>15</v>
       </c>
-      <c r="S1" s="82">
+      <c r="S1" s="67">
         <v>16</v>
       </c>
-      <c r="T1" s="82">
+      <c r="T1" s="67">
         <v>17</v>
       </c>
-      <c r="U1" s="82">
+      <c r="U1" s="67">
         <v>18</v>
       </c>
-      <c r="V1" s="82">
+      <c r="V1" s="67">
         <v>19</v>
       </c>
-      <c r="W1" s="82">
+      <c r="W1" s="67">
         <v>20</v>
       </c>
-      <c r="X1" s="82">
+      <c r="X1" s="67">
         <v>21</v>
       </c>
-      <c r="Y1" s="82">
+      <c r="Y1" s="67">
         <v>22</v>
       </c>
-      <c r="Z1" s="82">
+      <c r="Z1" s="67">
         <v>23</v>
       </c>
-      <c r="AA1" s="82">
+      <c r="AA1" s="67">
         <v>24</v>
       </c>
-      <c r="AB1" s="82">
+      <c r="AB1" s="67">
         <v>25</v>
       </c>
-      <c r="AC1" s="82">
+      <c r="AC1" s="67">
         <v>26</v>
       </c>
-      <c r="AD1" s="82">
+      <c r="AD1" s="67">
         <v>27</v>
       </c>
-      <c r="AE1" s="83">
+      <c r="AE1" s="68">
         <v>28</v>
       </c>
       <c r="AF1" s="35"/>
@@ -10807,19 +10977,23 @@
         <v>42</v>
       </c>
       <c r="I31" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J31" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="L31" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="M31" s="36"/>
-      <c r="N31" s="36"/>
+        <v>43</v>
+      </c>
+      <c r="M31" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="N31" s="36" t="s">
+        <v>143</v>
+      </c>
       <c r="O31" s="36"/>
       <c r="P31" s="36"/>
       <c r="Q31" s="36"/>
@@ -11083,7 +11257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A04060-45CA-49C0-9E02-FCC68C03B3FB}">
   <dimension ref="A1:AQ43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -11096,133 +11270,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="84" t="s">
+      <c r="A1" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="81">
-        <v>1</v>
-      </c>
-      <c r="E1" s="82">
+      <c r="C1" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="66">
+        <v>1</v>
+      </c>
+      <c r="E1" s="67">
         <v>2</v>
       </c>
-      <c r="F1" s="82">
+      <c r="F1" s="67">
         <v>3</v>
       </c>
-      <c r="G1" s="82">
+      <c r="G1" s="67">
         <v>4</v>
       </c>
-      <c r="H1" s="82">
+      <c r="H1" s="67">
         <v>5</v>
       </c>
-      <c r="I1" s="82">
+      <c r="I1" s="67">
         <v>6</v>
       </c>
-      <c r="J1" s="82">
+      <c r="J1" s="67">
         <v>7</v>
       </c>
-      <c r="K1" s="82">
+      <c r="K1" s="67">
         <v>8</v>
       </c>
-      <c r="L1" s="82">
+      <c r="L1" s="67">
         <v>9</v>
       </c>
-      <c r="M1" s="82">
+      <c r="M1" s="67">
         <v>10</v>
       </c>
-      <c r="N1" s="82">
+      <c r="N1" s="67">
         <v>11</v>
       </c>
-      <c r="O1" s="82">
+      <c r="O1" s="67">
         <v>12</v>
       </c>
-      <c r="P1" s="82">
+      <c r="P1" s="67">
         <v>13</v>
       </c>
-      <c r="Q1" s="82">
+      <c r="Q1" s="67">
         <v>14</v>
       </c>
-      <c r="R1" s="82">
+      <c r="R1" s="67">
         <v>15</v>
       </c>
-      <c r="S1" s="82">
+      <c r="S1" s="67">
         <v>16</v>
       </c>
-      <c r="T1" s="82">
+      <c r="T1" s="67">
         <v>17</v>
       </c>
-      <c r="U1" s="82">
+      <c r="U1" s="67">
         <v>18</v>
       </c>
-      <c r="V1" s="82">
+      <c r="V1" s="67">
         <v>19</v>
       </c>
-      <c r="W1" s="82">
+      <c r="W1" s="67">
         <v>20</v>
       </c>
-      <c r="X1" s="82">
+      <c r="X1" s="67">
         <v>21</v>
       </c>
-      <c r="Y1" s="82">
+      <c r="Y1" s="67">
         <v>22</v>
       </c>
-      <c r="Z1" s="82">
+      <c r="Z1" s="67">
         <v>23</v>
       </c>
-      <c r="AA1" s="82">
+      <c r="AA1" s="67">
         <v>24</v>
       </c>
-      <c r="AB1" s="82">
+      <c r="AB1" s="67">
         <v>25</v>
       </c>
-      <c r="AC1" s="82">
+      <c r="AC1" s="67">
         <v>26</v>
       </c>
-      <c r="AD1" s="82">
+      <c r="AD1" s="67">
         <v>27</v>
       </c>
-      <c r="AE1" s="82">
+      <c r="AE1" s="67">
         <v>28</v>
       </c>
-      <c r="AF1" s="82">
+      <c r="AF1" s="67">
         <v>29</v>
       </c>
-      <c r="AG1" s="82">
+      <c r="AG1" s="67">
         <v>30</v>
       </c>
-      <c r="AH1" s="82">
+      <c r="AH1" s="67">
         <v>31</v>
       </c>
-      <c r="AI1" s="82">
+      <c r="AI1" s="67">
         <v>32</v>
       </c>
-      <c r="AJ1" s="82">
+      <c r="AJ1" s="67">
         <v>33</v>
       </c>
-      <c r="AK1" s="82">
+      <c r="AK1" s="67">
         <v>34</v>
       </c>
-      <c r="AL1" s="82">
+      <c r="AL1" s="67">
         <v>35</v>
       </c>
-      <c r="AM1" s="82">
+      <c r="AM1" s="67">
         <v>36</v>
       </c>
-      <c r="AN1" s="82">
+      <c r="AN1" s="67">
         <v>37</v>
       </c>
-      <c r="AO1" s="82">
+      <c r="AO1" s="67">
         <v>38</v>
       </c>
-      <c r="AP1" s="82">
+      <c r="AP1" s="67">
         <v>39</v>
       </c>
-      <c r="AQ1" s="83">
+      <c r="AQ1" s="68">
         <v>40</v>
       </c>
     </row>
@@ -11447,7 +11621,7 @@
       <c r="B9" s="40">
         <v>1</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="70" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="44" t="s">
@@ -12260,7 +12434,7 @@
       <c r="B33" s="40">
         <v>1</v>
       </c>
-      <c r="C33" s="85"/>
+      <c r="C33" s="70"/>
       <c r="D33" s="44" t="s">
         <v>41</v>
       </c>
@@ -12476,7 +12650,7 @@
       <c r="B40" s="40">
         <v>1</v>
       </c>
-      <c r="C40" s="85" t="s">
+      <c r="C40" s="70" t="s">
         <v>138</v>
       </c>
       <c r="D40" s="44" t="s">
@@ -12592,4 +12766,1210 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D895FAFD-06CA-4987-9579-0AFB8A1491E7}">
+  <dimension ref="A1:AE79"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19:N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" customWidth="1"/>
+    <col min="4" max="21" width="2.7265625" customWidth="1"/>
+    <col min="22" max="31" width="8.6328125" customWidth="1"/>
+    <col min="33" max="33" width="17.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A1" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="66">
+        <v>1</v>
+      </c>
+      <c r="E1" s="67">
+        <v>2</v>
+      </c>
+      <c r="F1" s="67">
+        <v>3</v>
+      </c>
+      <c r="G1" s="67">
+        <v>4</v>
+      </c>
+      <c r="H1" s="67">
+        <v>5</v>
+      </c>
+      <c r="I1" s="67">
+        <v>6</v>
+      </c>
+      <c r="J1" s="67">
+        <v>7</v>
+      </c>
+      <c r="K1" s="67">
+        <v>8</v>
+      </c>
+      <c r="L1" s="67">
+        <v>9</v>
+      </c>
+      <c r="M1" s="67">
+        <v>10</v>
+      </c>
+      <c r="N1" s="67">
+        <v>11</v>
+      </c>
+      <c r="O1" s="67">
+        <v>12</v>
+      </c>
+      <c r="P1" s="67">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="67">
+        <v>14</v>
+      </c>
+      <c r="R1" s="67">
+        <v>15</v>
+      </c>
+      <c r="S1" s="67">
+        <v>16</v>
+      </c>
+      <c r="T1" s="67">
+        <v>17</v>
+      </c>
+      <c r="U1" s="68">
+        <v>18</v>
+      </c>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
+      <c r="AA1" s="86"/>
+      <c r="AB1" s="86"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="40">
+        <v>1</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" t="s">
+        <v>143</v>
+      </c>
+      <c r="U2" s="38"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I3" t="s">
+        <v>143</v>
+      </c>
+      <c r="U3" s="38"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="40">
+        <v>1</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" t="s">
+        <v>143</v>
+      </c>
+      <c r="U4" s="38"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" t="s">
+        <v>143</v>
+      </c>
+      <c r="U5" s="38"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="40">
+        <v>1</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>144</v>
+      </c>
+      <c r="L6" t="s">
+        <v>143</v>
+      </c>
+      <c r="U6" s="38"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="41">
+        <v>1</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="40">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U8" s="38"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="40">
+        <v>1</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U9" s="38"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" s="40">
+        <v>1</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U10" s="38"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A11" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" s="40">
+        <v>1</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U11" s="38"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="40">
+        <v>1</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U12" s="38"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="40">
+        <v>1</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="I13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U13" s="38"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="40">
+        <v>1</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U14" s="38"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="40">
+        <v>1</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>42</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U15" s="38"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="40">
+        <v>2</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="L16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="38"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A17" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="40">
+        <v>1</v>
+      </c>
+      <c r="D17" s="44"/>
+      <c r="M17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>144</v>
+      </c>
+      <c r="R17" t="s">
+        <v>143</v>
+      </c>
+      <c r="U17" s="38"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A18" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="41">
+        <v>3</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="R18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="S18" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="T18" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="U18" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="V18" s="44"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A19" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="40">
+        <v>1</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>144</v>
+      </c>
+      <c r="H19" t="s">
+        <v>143</v>
+      </c>
+      <c r="U19" s="38"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A20" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="40">
+        <v>1</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>143</v>
+      </c>
+      <c r="U20" s="38"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A21" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="40">
+        <v>1</v>
+      </c>
+      <c r="D21" s="44"/>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" t="s">
+        <v>143</v>
+      </c>
+      <c r="U21" s="38"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A22" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="41">
+        <v>2</v>
+      </c>
+      <c r="C22" s="36"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="N22" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="36"/>
+      <c r="U22" s="39"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A23" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="40">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="U23" s="38"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A24" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" s="40">
+        <v>1</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A25" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="41">
+        <v>3</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="L25" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="39"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A26" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" s="41">
+        <v>1</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="39"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+    </row>
+    <row r="33" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+    </row>
+    <row r="34" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+    </row>
+    <row r="35" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+    </row>
+    <row r="36" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+    </row>
+    <row r="37" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+    </row>
+    <row r="38" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC38" s="1"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+    </row>
+    <row r="39" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC39" s="1"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+    </row>
+    <row r="40" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC40" s="1"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+    </row>
+    <row r="41" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC41" s="1"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+    </row>
+    <row r="42" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+    </row>
+    <row r="43" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
+      <c r="AE43" s="1"/>
+    </row>
+    <row r="44" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+    </row>
+    <row r="45" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+    </row>
+    <row r="46" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC46" s="1"/>
+      <c r="AD46" s="1"/>
+      <c r="AE46" s="1"/>
+    </row>
+    <row r="47" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+    </row>
+    <row r="48" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC48" s="1"/>
+      <c r="AD48" s="1"/>
+      <c r="AE48" s="1"/>
+    </row>
+    <row r="49" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+    </row>
+    <row r="50" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC50" s="1"/>
+      <c r="AD50" s="1"/>
+      <c r="AE50" s="1"/>
+    </row>
+    <row r="51" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+    </row>
+    <row r="52" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+    </row>
+    <row r="53" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC53" s="1"/>
+      <c r="AD53" s="1"/>
+      <c r="AE53" s="1"/>
+    </row>
+    <row r="54" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC54" s="1"/>
+      <c r="AD54" s="1"/>
+      <c r="AE54" s="1"/>
+    </row>
+    <row r="55" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC55" s="1"/>
+      <c r="AD55" s="1"/>
+      <c r="AE55" s="1"/>
+    </row>
+    <row r="56" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+    </row>
+    <row r="57" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC57" s="1"/>
+      <c r="AD57" s="1"/>
+      <c r="AE57" s="1"/>
+    </row>
+    <row r="58" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC58" s="1"/>
+      <c r="AD58" s="1"/>
+      <c r="AE58" s="1"/>
+    </row>
+    <row r="59" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC59" s="1"/>
+      <c r="AD59" s="1"/>
+      <c r="AE59" s="1"/>
+    </row>
+    <row r="60" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+    </row>
+    <row r="61" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC61" s="1"/>
+      <c r="AD61" s="1"/>
+      <c r="AE61" s="1"/>
+    </row>
+    <row r="62" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1"/>
+      <c r="AE62" s="1"/>
+    </row>
+    <row r="63" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC63" s="1"/>
+      <c r="AD63" s="1"/>
+      <c r="AE63" s="1"/>
+    </row>
+    <row r="64" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
+      <c r="AE64" s="1"/>
+    </row>
+    <row r="65" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
+      <c r="AE65" s="1"/>
+    </row>
+    <row r="66" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+    </row>
+    <row r="67" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+    </row>
+    <row r="68" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
+      <c r="AE68" s="1"/>
+    </row>
+    <row r="69" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AE69" s="1"/>
+    </row>
+    <row r="70" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+    </row>
+    <row r="71" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AE71" s="1"/>
+    </row>
+    <row r="72" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC72" s="1"/>
+      <c r="AD72" s="1"/>
+      <c r="AE72" s="1"/>
+    </row>
+    <row r="73" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC73" s="1"/>
+      <c r="AD73" s="1"/>
+      <c r="AE73" s="1"/>
+    </row>
+    <row r="74" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC74" s="1"/>
+      <c r="AD74" s="1"/>
+      <c r="AE74" s="1"/>
+    </row>
+    <row r="75" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC75" s="1"/>
+      <c r="AD75" s="1"/>
+      <c r="AE75" s="1"/>
+    </row>
+    <row r="76" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC76" s="1"/>
+      <c r="AD76" s="1"/>
+      <c r="AE76" s="1"/>
+    </row>
+    <row r="77" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC77" s="1"/>
+      <c r="AD77" s="1"/>
+      <c r="AE77" s="1"/>
+    </row>
+    <row r="78" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC78" s="1"/>
+      <c r="AD78" s="1"/>
+      <c r="AE78" s="1"/>
+    </row>
+    <row r="79" spans="29:31" x14ac:dyDescent="0.35">
+      <c r="AC79" s="1"/>
+      <c r="AD79" s="1"/>
+      <c r="AE79" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>